<commit_message>
added dietel examples to project, worked on 640 ch5 ex
</commit_message>
<xml_diff>
--- a/csulb-is-601/exams/exam3/IS 601 Module 3.xlsx
+++ b/csulb-is-601/exams/exam3/IS 601 Module 3.xlsx
@@ -1,32 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\User Archive\Spheres\BIZ\_education\Data Science\Formal\CSULB MSIS\IS 640\learning-python\csulb-is-601\homework\ch10\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\User Archive\Spheres\BIZ\_education\Data Science\Formal\CSULB MSIS\IS 640\learning-python\csulb-is-601\exams\exam3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E7FF6D2-D2DB-47F3-8F60-D94437E1950B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0E960FC-6976-4E4E-A95F-6DD73A41FFBA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{CA8A5116-5F6B-4D16-9D61-36C317C3C722}"/>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15600" tabRatio="753" activeTab="1" xr2:uid="{39856AD9-BEBD-4883-887C-DCC6FA625468}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="753" activeTab="4" xr2:uid="{39856AD9-BEBD-4883-887C-DCC6FA625468}"/>
   </bookViews>
   <sheets>
     <sheet name="Module 3 HW" sheetId="19" r:id="rId1"/>
-    <sheet name="Hypo Test known Sigma" sheetId="23" r:id="rId2"/>
-    <sheet name="Hypo Test unknown Sigma" sheetId="22" r:id="rId3"/>
+    <sheet name="1-sample Hypo Test known Sigma" sheetId="23" r:id="rId2"/>
+    <sheet name="1-sampleHypo Test unknown Sigma" sheetId="22" r:id="rId3"/>
     <sheet name="Type II Error" sheetId="24" r:id="rId4"/>
-    <sheet name="z-Table" sheetId="20" r:id="rId5"/>
-    <sheet name="t-Table" sheetId="21" r:id="rId6"/>
+    <sheet name="11042020 group exercise" sheetId="25" r:id="rId5"/>
+    <sheet name="z-Table" sheetId="20" r:id="rId6"/>
+    <sheet name="t-Table" sheetId="21" r:id="rId7"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId7"/>
+    <externalReference r:id="rId8"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_hypTest_known_sigma">'Hypo Test known Sigma'!$K$123:$P$162</definedName>
-    <definedName name="_hypTest_unknown_sigma">'Hypo Test unknown Sigma'!$K$289:$AC$339</definedName>
+    <definedName name="_hypTest_known_sigma">'1-sample Hypo Test known Sigma'!$K$123:$P$162</definedName>
+    <definedName name="_hypTest_unknown_sigma">'1-sampleHypo Test unknown Sigma'!$K$289:$AC$339</definedName>
     <definedName name="_randVar">'[1]When to use what formula'!$J$10</definedName>
     <definedName name="_success">'[1]When to use what formula'!$J$13</definedName>
     <definedName name="_t_table">'t-Table'!$A$1</definedName>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="178">
   <si>
     <t>Ex5.</t>
   </si>
@@ -455,12 +455,6 @@
     <t>It is reasonable to conclude that the mean number of customers using the self-checkout system is more than 100 per day</t>
   </si>
   <si>
-    <t>Hypo Test known Sigma</t>
-  </si>
-  <si>
-    <t>Hypo Test unknown Sigma</t>
-  </si>
-  <si>
     <t>Type II Error</t>
   </si>
   <si>
@@ -477,20 +471,139 @@
   </si>
   <si>
     <t>Ch. 10: 11, 13, 17, 19, 33, 37, 41</t>
+  </si>
+  <si>
+    <t>Hypo Test known Sigma 1-sample</t>
+  </si>
+  <si>
+    <t>Hypo Test unknown Sigma 1-sample</t>
+  </si>
+  <si>
+    <t>Step 1:</t>
+  </si>
+  <si>
+    <t>Step 2:</t>
+  </si>
+  <si>
+    <t>Step 3:</t>
+  </si>
+  <si>
+    <t>Step 4:</t>
+  </si>
+  <si>
+    <t>Ex41</t>
+  </si>
+  <si>
+    <t>Many grocery stores and large retailers such as Kroger and Walmart have installed self-checked out systems so shoppers can scan their own items and cash out themselves. How do customers like this service and how often do they use it? Listed below is the number of customers using the services for a sample of 15 days at a Walmart location.
+Is it reasonable to conclude that the mean number of customers using the self-checkout system is more than 100 per day? Use 0.05 significance level.</t>
+  </si>
+  <si>
+    <t>Population Mean (mu)</t>
+  </si>
+  <si>
+    <t>Samples(n)</t>
+  </si>
+  <si>
+    <t>Sample mean (Xbar)</t>
+  </si>
+  <si>
+    <t>Sample Standard Deviation (S)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alpha </t>
+  </si>
+  <si>
+    <t>unknown sigma</t>
+  </si>
+  <si>
+    <t>mu &lt;= 100</t>
+  </si>
+  <si>
+    <t>mu &gt; 100</t>
+  </si>
+  <si>
+    <t>right tailed</t>
+  </si>
+  <si>
+    <t>computed t-value</t>
+  </si>
+  <si>
+    <t>&lt; p &lt;</t>
+  </si>
+  <si>
+    <t>Reject H0</t>
+  </si>
+  <si>
+    <t>It is reasonable to conclude that the mean number of customers using the self-checkout system is more than 100 per day.</t>
+  </si>
+  <si>
+    <t>p &lt; alpha</t>
+  </si>
+  <si>
+    <t>dummy</t>
+  </si>
+  <si>
+    <t>Hypothesized Mean</t>
+  </si>
+  <si>
+    <t>t-Test: One-Sample</t>
+  </si>
+  <si>
+    <t>Excel Data Analysis Method</t>
+  </si>
+  <si>
+    <t>Data Analysis Method</t>
+  </si>
+  <si>
+    <t>self-ckout</t>
+  </si>
+  <si>
+    <t>=COUNT(B13:B27)</t>
+  </si>
+  <si>
+    <t>=AVERAGE(B13:B27)</t>
+  </si>
+  <si>
+    <t>=STDEV.S(B13:B27)</t>
+  </si>
+  <si>
+    <t>Group 5 - p-value approach</t>
+  </si>
+  <si>
+    <t>H0:</t>
+  </si>
+  <si>
+    <t>Ha:</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>=1-T.DIST(M20,M5-1,TRUE)</t>
+  </si>
+  <si>
+    <t>=(M20-M4)/(M21/SQRT(M5))</t>
+  </si>
+  <si>
+    <t>=M5-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data &gt; Data Analysis &gt; </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="170" formatCode="0.000"/>
-    <numFmt numFmtId="171" formatCode="0.0000"/>
-    <numFmt numFmtId="172" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="170" formatCode="0.0000000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="9"/>
       <color theme="1"/>
@@ -532,8 +645,19 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -546,8 +670,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -575,13 +705,84 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -596,7 +797,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -609,24 +810,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="171" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -639,8 +840,8 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -652,34 +853,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -688,19 +886,104 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="170" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -969,6 +1252,55 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>154278</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>117895</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98A5D87A-49AE-4C0B-9736-19EFF177F71C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9216445" y="3588644"/>
+          <a:ext cx="3226426" cy="2130219"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1480,45 +1812,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4041B246-1F07-42D3-8525-F84CB90D5CCE}">
-  <dimension ref="C1:D9"/>
+  <dimension ref="C1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C1" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C2" s="2" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="D2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C3" s="2" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="D3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C4" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="3:4" x14ac:dyDescent="0.2">
@@ -1526,18 +1857,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="D7" t="s">
+    <row r="13" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="D8" t="s">
+    <row r="14" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="D14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="D9" t="s">
+    <row r="15" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1551,9 +1882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCC6B74C-CB07-4DDA-9CF8-5466436436E1}">
   <dimension ref="A1:P162"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="1">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="P71" sqref="P71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1575,16 +1905,16 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
       <c r="K2" s="1">
         <v>1</v>
       </c>
@@ -1594,21 +1924,21 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
       <c r="M3" s="2" t="s">
         <v>18</v>
       </c>
       <c r="N3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="39">
+      <c r="O3" s="38">
         <v>60000</v>
       </c>
       <c r="P3" t="s">
@@ -1617,41 +1947,41 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="50"/>
       <c r="M4" s="2" t="s">
         <v>19</v>
       </c>
       <c r="N4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O4" s="39">
+      <c r="O4" s="38">
         <v>5000</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
-      <c r="B5" s="38"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="50"/>
       <c r="M5" s="2" t="s">
         <v>20</v>
       </c>
       <c r="N5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="O5" s="39">
+      <c r="O5" s="38">
         <v>59500</v>
       </c>
       <c r="P5" t="s">
@@ -1660,21 +1990,21 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
-      <c r="B6" s="38"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="50"/>
+      <c r="I6" s="50"/>
       <c r="M6" s="2" t="s">
         <v>22</v>
       </c>
       <c r="N6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="O6" s="39">
+      <c r="O6" s="38">
         <v>48</v>
       </c>
       <c r="P6" t="s">
@@ -1683,53 +2013,53 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
-      <c r="B7" s="38"/>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="50"/>
       <c r="M7" s="2" t="s">
         <v>42</v>
       </c>
       <c r="N7" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="O7" s="40"/>
+      <c r="O7" s="39"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
-      <c r="B8" s="38"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="38"/>
+      <c r="B8" s="50"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="50"/>
+      <c r="H8" s="50"/>
+      <c r="I8" s="50"/>
       <c r="M8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="O8" s="39">
+      <c r="O8" s="38">
         <v>0.95</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="38"/>
+      <c r="B9" s="50"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="50"/>
+      <c r="I9" s="50"/>
       <c r="M9" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="O9" s="39" t="s">
+      <c r="O9" s="38" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1751,7 +2081,7 @@
       <c r="N10" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="O10" s="41">
+      <c r="O10" s="40">
         <f>1-O8</f>
         <v>5.0000000000000044E-2</v>
       </c>
@@ -2078,7 +2408,7 @@
       <c r="N31" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="O31" s="42">
+      <c r="O31" s="41">
         <f>_xlfn.NORM.S.DIST(O30,TRUE)-0.5</f>
         <v>0.25490290632569057</v>
       </c>
@@ -2160,16 +2490,16 @@
       <c r="A42" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B42" s="38" t="s">
+      <c r="B42" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="C42" s="38"/>
-      <c r="D42" s="38"/>
-      <c r="E42" s="38"/>
-      <c r="F42" s="38"/>
-      <c r="G42" s="38"/>
-      <c r="H42" s="38"/>
-      <c r="I42" s="38"/>
+      <c r="C42" s="50"/>
+      <c r="D42" s="50"/>
+      <c r="E42" s="50"/>
+      <c r="F42" s="50"/>
+      <c r="G42" s="50"/>
+      <c r="H42" s="50"/>
+      <c r="I42" s="50"/>
       <c r="K42" s="1">
         <v>1</v>
       </c>
@@ -2179,21 +2509,21 @@
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
-      <c r="B43" s="38"/>
-      <c r="C43" s="38"/>
-      <c r="D43" s="38"/>
-      <c r="E43" s="38"/>
-      <c r="F43" s="38"/>
-      <c r="G43" s="38"/>
-      <c r="H43" s="38"/>
-      <c r="I43" s="38"/>
+      <c r="B43" s="50"/>
+      <c r="C43" s="50"/>
+      <c r="D43" s="50"/>
+      <c r="E43" s="50"/>
+      <c r="F43" s="50"/>
+      <c r="G43" s="50"/>
+      <c r="H43" s="50"/>
+      <c r="I43" s="50"/>
       <c r="M43" s="2" t="s">
         <v>18</v>
       </c>
       <c r="N43" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O43" s="39">
+      <c r="O43" s="38">
         <v>6.8</v>
       </c>
       <c r="P43" t="s">
@@ -2202,41 +2532,41 @@
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
-      <c r="B44" s="38"/>
-      <c r="C44" s="38"/>
-      <c r="D44" s="38"/>
-      <c r="E44" s="38"/>
-      <c r="F44" s="38"/>
-      <c r="G44" s="38"/>
-      <c r="H44" s="38"/>
-      <c r="I44" s="38"/>
+      <c r="B44" s="50"/>
+      <c r="C44" s="50"/>
+      <c r="D44" s="50"/>
+      <c r="E44" s="50"/>
+      <c r="F44" s="50"/>
+      <c r="G44" s="50"/>
+      <c r="H44" s="50"/>
+      <c r="I44" s="50"/>
       <c r="M44" s="2" t="s">
         <v>19</v>
       </c>
       <c r="N44" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O44" s="39">
+      <c r="O44" s="38">
         <v>1.8</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
-      <c r="B45" s="38"/>
-      <c r="C45" s="38"/>
-      <c r="D45" s="38"/>
-      <c r="E45" s="38"/>
-      <c r="F45" s="38"/>
-      <c r="G45" s="38"/>
-      <c r="H45" s="38"/>
-      <c r="I45" s="38"/>
+      <c r="B45" s="50"/>
+      <c r="C45" s="50"/>
+      <c r="D45" s="50"/>
+      <c r="E45" s="50"/>
+      <c r="F45" s="50"/>
+      <c r="G45" s="50"/>
+      <c r="H45" s="50"/>
+      <c r="I45" s="50"/>
       <c r="M45" s="2" t="s">
         <v>20</v>
       </c>
       <c r="N45" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="O45" s="39">
+      <c r="O45" s="38">
         <v>6.2</v>
       </c>
       <c r="P45" t="s">
@@ -2245,21 +2575,21 @@
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
-      <c r="B46" s="38"/>
-      <c r="C46" s="38"/>
-      <c r="D46" s="38"/>
-      <c r="E46" s="38"/>
-      <c r="F46" s="38"/>
-      <c r="G46" s="38"/>
-      <c r="H46" s="38"/>
-      <c r="I46" s="38"/>
+      <c r="B46" s="50"/>
+      <c r="C46" s="50"/>
+      <c r="D46" s="50"/>
+      <c r="E46" s="50"/>
+      <c r="F46" s="50"/>
+      <c r="G46" s="50"/>
+      <c r="H46" s="50"/>
+      <c r="I46" s="50"/>
       <c r="M46" s="2" t="s">
         <v>22</v>
       </c>
       <c r="N46" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="O46" s="39">
+      <c r="O46" s="38">
         <v>36</v>
       </c>
       <c r="P46" t="s">
@@ -2268,53 +2598,53 @@
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47" s="1"/>
-      <c r="B47" s="38"/>
-      <c r="C47" s="38"/>
-      <c r="D47" s="38"/>
-      <c r="E47" s="38"/>
-      <c r="F47" s="38"/>
-      <c r="G47" s="38"/>
-      <c r="H47" s="38"/>
-      <c r="I47" s="38"/>
+      <c r="B47" s="50"/>
+      <c r="C47" s="50"/>
+      <c r="D47" s="50"/>
+      <c r="E47" s="50"/>
+      <c r="F47" s="50"/>
+      <c r="G47" s="50"/>
+      <c r="H47" s="50"/>
+      <c r="I47" s="50"/>
       <c r="M47" s="2" t="s">
         <v>42</v>
       </c>
       <c r="N47" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="O47" s="40"/>
+      <c r="O47" s="39"/>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48" s="1"/>
-      <c r="B48" s="38"/>
-      <c r="C48" s="38"/>
-      <c r="D48" s="38"/>
-      <c r="E48" s="38"/>
-      <c r="F48" s="38"/>
-      <c r="G48" s="38"/>
-      <c r="H48" s="38"/>
-      <c r="I48" s="38"/>
+      <c r="B48" s="50"/>
+      <c r="C48" s="50"/>
+      <c r="D48" s="50"/>
+      <c r="E48" s="50"/>
+      <c r="F48" s="50"/>
+      <c r="G48" s="50"/>
+      <c r="H48" s="50"/>
+      <c r="I48" s="50"/>
       <c r="M48" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="O48" s="39">
+      <c r="O48" s="38">
         <v>0.95</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A49" s="1"/>
-      <c r="B49" s="38"/>
-      <c r="C49" s="38"/>
-      <c r="D49" s="38"/>
-      <c r="E49" s="38"/>
-      <c r="F49" s="38"/>
-      <c r="G49" s="38"/>
-      <c r="H49" s="38"/>
-      <c r="I49" s="38"/>
+      <c r="B49" s="50"/>
+      <c r="C49" s="50"/>
+      <c r="D49" s="50"/>
+      <c r="E49" s="50"/>
+      <c r="F49" s="50"/>
+      <c r="G49" s="50"/>
+      <c r="H49" s="50"/>
+      <c r="I49" s="50"/>
       <c r="M49" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="O49" s="39" t="s">
+      <c r="O49" s="38" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2336,7 +2666,7 @@
       <c r="N50" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="O50" s="41">
+      <c r="O50" s="40">
         <f>1-O48</f>
         <v>5.0000000000000044E-2</v>
       </c>
@@ -2661,7 +2991,7 @@
       <c r="N71" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="O71" s="42">
+      <c r="O71" s="41">
         <f>_xlfn.NORM.S.DIST(O70,TRUE)-0.5</f>
         <v>0.47724986805182079</v>
       </c>
@@ -2743,16 +3073,16 @@
       <c r="A83" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B83" s="38" t="s">
+      <c r="B83" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="C83" s="38"/>
-      <c r="D83" s="38"/>
-      <c r="E83" s="38"/>
-      <c r="F83" s="38"/>
-      <c r="G83" s="38"/>
-      <c r="H83" s="38"/>
-      <c r="I83" s="38"/>
+      <c r="C83" s="50"/>
+      <c r="D83" s="50"/>
+      <c r="E83" s="50"/>
+      <c r="F83" s="50"/>
+      <c r="G83" s="50"/>
+      <c r="H83" s="50"/>
+      <c r="I83" s="50"/>
       <c r="K83" s="1">
         <v>1</v>
       </c>
@@ -2762,21 +3092,21 @@
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A84" s="1"/>
-      <c r="B84" s="38"/>
-      <c r="C84" s="38"/>
-      <c r="D84" s="38"/>
-      <c r="E84" s="38"/>
-      <c r="F84" s="38"/>
-      <c r="G84" s="38"/>
-      <c r="H84" s="38"/>
-      <c r="I84" s="38"/>
+      <c r="B84" s="50"/>
+      <c r="C84" s="50"/>
+      <c r="D84" s="50"/>
+      <c r="E84" s="50"/>
+      <c r="F84" s="50"/>
+      <c r="G84" s="50"/>
+      <c r="H84" s="50"/>
+      <c r="I84" s="50"/>
       <c r="M84" s="2" t="s">
         <v>18</v>
       </c>
       <c r="N84" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O84" s="39">
+      <c r="O84" s="38">
         <v>45000</v>
       </c>
       <c r="P84" t="s">
@@ -2785,41 +3115,41 @@
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A85" s="1"/>
-      <c r="B85" s="38"/>
-      <c r="C85" s="38"/>
-      <c r="D85" s="38"/>
-      <c r="E85" s="38"/>
-      <c r="F85" s="38"/>
-      <c r="G85" s="38"/>
-      <c r="H85" s="38"/>
-      <c r="I85" s="38"/>
+      <c r="B85" s="50"/>
+      <c r="C85" s="50"/>
+      <c r="D85" s="50"/>
+      <c r="E85" s="50"/>
+      <c r="F85" s="50"/>
+      <c r="G85" s="50"/>
+      <c r="H85" s="50"/>
+      <c r="I85" s="50"/>
       <c r="M85" s="2" t="s">
         <v>19</v>
       </c>
       <c r="N85" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O85" s="39">
+      <c r="O85" s="38">
         <v>3000</v>
       </c>
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A86" s="1"/>
-      <c r="B86" s="38"/>
-      <c r="C86" s="38"/>
-      <c r="D86" s="38"/>
-      <c r="E86" s="38"/>
-      <c r="F86" s="38"/>
-      <c r="G86" s="38"/>
-      <c r="H86" s="38"/>
-      <c r="I86" s="38"/>
+      <c r="B86" s="50"/>
+      <c r="C86" s="50"/>
+      <c r="D86" s="50"/>
+      <c r="E86" s="50"/>
+      <c r="F86" s="50"/>
+      <c r="G86" s="50"/>
+      <c r="H86" s="50"/>
+      <c r="I86" s="50"/>
       <c r="M86" s="2" t="s">
         <v>20</v>
       </c>
       <c r="N86" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="O86" s="39">
+      <c r="O86" s="38">
         <v>45500</v>
       </c>
       <c r="P86" t="s">
@@ -2828,21 +3158,21 @@
     </row>
     <row r="87" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A87" s="1"/>
-      <c r="B87" s="38"/>
-      <c r="C87" s="38"/>
-      <c r="D87" s="38"/>
-      <c r="E87" s="38"/>
-      <c r="F87" s="38"/>
-      <c r="G87" s="38"/>
-      <c r="H87" s="38"/>
-      <c r="I87" s="38"/>
+      <c r="B87" s="50"/>
+      <c r="C87" s="50"/>
+      <c r="D87" s="50"/>
+      <c r="E87" s="50"/>
+      <c r="F87" s="50"/>
+      <c r="G87" s="50"/>
+      <c r="H87" s="50"/>
+      <c r="I87" s="50"/>
       <c r="M87" s="2" t="s">
         <v>22</v>
       </c>
       <c r="N87" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="O87" s="39">
+      <c r="O87" s="38">
         <v>120</v>
       </c>
       <c r="P87" t="s">
@@ -2851,53 +3181,53 @@
     </row>
     <row r="88" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A88" s="1"/>
-      <c r="B88" s="38"/>
-      <c r="C88" s="38"/>
-      <c r="D88" s="38"/>
-      <c r="E88" s="38"/>
-      <c r="F88" s="38"/>
-      <c r="G88" s="38"/>
-      <c r="H88" s="38"/>
-      <c r="I88" s="38"/>
+      <c r="B88" s="50"/>
+      <c r="C88" s="50"/>
+      <c r="D88" s="50"/>
+      <c r="E88" s="50"/>
+      <c r="F88" s="50"/>
+      <c r="G88" s="50"/>
+      <c r="H88" s="50"/>
+      <c r="I88" s="50"/>
       <c r="M88" s="2" t="s">
         <v>42</v>
       </c>
       <c r="N88" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="O88" s="40"/>
+      <c r="O88" s="39"/>
     </row>
     <row r="89" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A89" s="1"/>
-      <c r="B89" s="38"/>
-      <c r="C89" s="38"/>
-      <c r="D89" s="38"/>
-      <c r="E89" s="38"/>
-      <c r="F89" s="38"/>
-      <c r="G89" s="38"/>
-      <c r="H89" s="38"/>
-      <c r="I89" s="38"/>
+      <c r="B89" s="50"/>
+      <c r="C89" s="50"/>
+      <c r="D89" s="50"/>
+      <c r="E89" s="50"/>
+      <c r="F89" s="50"/>
+      <c r="G89" s="50"/>
+      <c r="H89" s="50"/>
+      <c r="I89" s="50"/>
       <c r="M89" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="O89" s="39">
+      <c r="O89" s="38">
         <v>0.9</v>
       </c>
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A90" s="1"/>
-      <c r="B90" s="38"/>
-      <c r="C90" s="38"/>
-      <c r="D90" s="38"/>
-      <c r="E90" s="38"/>
-      <c r="F90" s="38"/>
-      <c r="G90" s="38"/>
-      <c r="H90" s="38"/>
-      <c r="I90" s="38"/>
+      <c r="B90" s="50"/>
+      <c r="C90" s="50"/>
+      <c r="D90" s="50"/>
+      <c r="E90" s="50"/>
+      <c r="F90" s="50"/>
+      <c r="G90" s="50"/>
+      <c r="H90" s="50"/>
+      <c r="I90" s="50"/>
       <c r="M90" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="O90" s="39" t="s">
+      <c r="O90" s="38" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2919,7 +3249,7 @@
       <c r="N91" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="O91" s="41">
+      <c r="O91" s="40">
         <f>1-O89</f>
         <v>9.9999999999999978E-2</v>
       </c>
@@ -3257,7 +3587,7 @@
       <c r="N113" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="O113" s="42">
+      <c r="O113" s="41">
         <f>_xlfn.NORM.S.DIST(O112,TRUE)-0.5</f>
         <v>0.46637503058037166</v>
       </c>
@@ -3362,16 +3692,16 @@
       <c r="A124" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B124" s="38" t="s">
+      <c r="B124" s="50" t="s">
         <v>117</v>
       </c>
-      <c r="C124" s="38"/>
-      <c r="D124" s="38"/>
-      <c r="E124" s="38"/>
-      <c r="F124" s="38"/>
-      <c r="G124" s="38"/>
-      <c r="H124" s="38"/>
-      <c r="I124" s="38"/>
+      <c r="C124" s="50"/>
+      <c r="D124" s="50"/>
+      <c r="E124" s="50"/>
+      <c r="F124" s="50"/>
+      <c r="G124" s="50"/>
+      <c r="H124" s="50"/>
+      <c r="I124" s="50"/>
       <c r="K124" s="1">
         <v>1</v>
       </c>
@@ -3381,21 +3711,21 @@
     </row>
     <row r="125" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A125" s="1"/>
-      <c r="B125" s="38"/>
-      <c r="C125" s="38"/>
-      <c r="D125" s="38"/>
-      <c r="E125" s="38"/>
-      <c r="F125" s="38"/>
-      <c r="G125" s="38"/>
-      <c r="H125" s="38"/>
-      <c r="I125" s="38"/>
+      <c r="B125" s="50"/>
+      <c r="C125" s="50"/>
+      <c r="D125" s="50"/>
+      <c r="E125" s="50"/>
+      <c r="F125" s="50"/>
+      <c r="G125" s="50"/>
+      <c r="H125" s="50"/>
+      <c r="I125" s="50"/>
       <c r="M125" s="2" t="s">
         <v>18</v>
       </c>
       <c r="N125" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O125" s="39">
+      <c r="O125" s="38">
         <v>10</v>
       </c>
       <c r="P125" t="s">
@@ -3404,41 +3734,41 @@
     </row>
     <row r="126" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A126" s="1"/>
-      <c r="B126" s="38"/>
-      <c r="C126" s="38"/>
-      <c r="D126" s="38"/>
-      <c r="E126" s="38"/>
-      <c r="F126" s="38"/>
-      <c r="G126" s="38"/>
-      <c r="H126" s="38"/>
-      <c r="I126" s="38"/>
+      <c r="B126" s="50"/>
+      <c r="C126" s="50"/>
+      <c r="D126" s="50"/>
+      <c r="E126" s="50"/>
+      <c r="F126" s="50"/>
+      <c r="G126" s="50"/>
+      <c r="H126" s="50"/>
+      <c r="I126" s="50"/>
       <c r="M126" s="2" t="s">
         <v>19</v>
       </c>
       <c r="N126" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O126" s="39">
+      <c r="O126" s="38">
         <v>2.8</v>
       </c>
     </row>
     <row r="127" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A127" s="1"/>
-      <c r="B127" s="38"/>
-      <c r="C127" s="38"/>
-      <c r="D127" s="38"/>
-      <c r="E127" s="38"/>
-      <c r="F127" s="38"/>
-      <c r="G127" s="38"/>
-      <c r="H127" s="38"/>
-      <c r="I127" s="38"/>
+      <c r="B127" s="50"/>
+      <c r="C127" s="50"/>
+      <c r="D127" s="50"/>
+      <c r="E127" s="50"/>
+      <c r="F127" s="50"/>
+      <c r="G127" s="50"/>
+      <c r="H127" s="50"/>
+      <c r="I127" s="50"/>
       <c r="M127" s="2" t="s">
         <v>20</v>
       </c>
       <c r="N127" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="O127" s="39">
+      <c r="O127" s="38">
         <v>9</v>
       </c>
       <c r="P127" t="s">
@@ -3447,21 +3777,21 @@
     </row>
     <row r="128" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A128" s="1"/>
-      <c r="B128" s="38"/>
-      <c r="C128" s="38"/>
-      <c r="D128" s="38"/>
-      <c r="E128" s="38"/>
-      <c r="F128" s="38"/>
-      <c r="G128" s="38"/>
-      <c r="H128" s="38"/>
-      <c r="I128" s="38"/>
+      <c r="B128" s="50"/>
+      <c r="C128" s="50"/>
+      <c r="D128" s="50"/>
+      <c r="E128" s="50"/>
+      <c r="F128" s="50"/>
+      <c r="G128" s="50"/>
+      <c r="H128" s="50"/>
+      <c r="I128" s="50"/>
       <c r="M128" s="2" t="s">
         <v>22</v>
       </c>
       <c r="N128" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="O128" s="39">
+      <c r="O128" s="38">
         <v>50</v>
       </c>
       <c r="P128" t="s">
@@ -3470,53 +3800,53 @@
     </row>
     <row r="129" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A129" s="1"/>
-      <c r="B129" s="38"/>
-      <c r="C129" s="38"/>
-      <c r="D129" s="38"/>
-      <c r="E129" s="38"/>
-      <c r="F129" s="38"/>
-      <c r="G129" s="38"/>
-      <c r="H129" s="38"/>
-      <c r="I129" s="38"/>
+      <c r="B129" s="50"/>
+      <c r="C129" s="50"/>
+      <c r="D129" s="50"/>
+      <c r="E129" s="50"/>
+      <c r="F129" s="50"/>
+      <c r="G129" s="50"/>
+      <c r="H129" s="50"/>
+      <c r="I129" s="50"/>
       <c r="M129" s="2" t="s">
         <v>42</v>
       </c>
       <c r="N129" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="O129" s="40"/>
+      <c r="O129" s="39"/>
     </row>
     <row r="130" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A130" s="1"/>
-      <c r="B130" s="38"/>
-      <c r="C130" s="38"/>
-      <c r="D130" s="38"/>
-      <c r="E130" s="38"/>
-      <c r="F130" s="38"/>
-      <c r="G130" s="38"/>
-      <c r="H130" s="38"/>
-      <c r="I130" s="38"/>
+      <c r="B130" s="50"/>
+      <c r="C130" s="50"/>
+      <c r="D130" s="50"/>
+      <c r="E130" s="50"/>
+      <c r="F130" s="50"/>
+      <c r="G130" s="50"/>
+      <c r="H130" s="50"/>
+      <c r="I130" s="50"/>
       <c r="M130" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="O130" s="39">
+      <c r="O130" s="38">
         <v>0.95</v>
       </c>
     </row>
     <row r="131" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A131" s="1"/>
-      <c r="B131" s="38"/>
-      <c r="C131" s="38"/>
-      <c r="D131" s="38"/>
-      <c r="E131" s="38"/>
-      <c r="F131" s="38"/>
-      <c r="G131" s="38"/>
-      <c r="H131" s="38"/>
-      <c r="I131" s="38"/>
+      <c r="B131" s="50"/>
+      <c r="C131" s="50"/>
+      <c r="D131" s="50"/>
+      <c r="E131" s="50"/>
+      <c r="F131" s="50"/>
+      <c r="G131" s="50"/>
+      <c r="H131" s="50"/>
+      <c r="I131" s="50"/>
       <c r="M131" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="O131" s="39" t="s">
+      <c r="O131" s="38" t="s">
         <v>36</v>
       </c>
     </row>
@@ -3538,7 +3868,7 @@
       <c r="N132" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="O132" s="41">
+      <c r="O132" s="40">
         <f>1-O130</f>
         <v>5.0000000000000044E-2</v>
       </c>
@@ -3875,7 +4205,7 @@
       <c r="N154" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="O154" s="42">
+      <c r="O154" s="41">
         <f>_xlfn.NORM.S.DIST(O153,TRUE)-0.5</f>
         <v>0.49429687366704933</v>
       </c>
@@ -3989,8 +4319,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECAE6B67-2380-4832-930E-4EB301EA776F}">
   <dimension ref="A1:AC339"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
+    <sheetView topLeftCell="A290" workbookViewId="0">
+      <selection activeCell="O320" sqref="O320"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4013,17 +4344,17 @@
       <c r="A2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
       <c r="K2" s="1">
         <v>1</v>
       </c>
@@ -4034,22 +4365,22 @@
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
       <c r="M3" s="2" t="s">
         <v>18</v>
       </c>
       <c r="N3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="39">
+      <c r="O3" s="38">
         <v>40</v>
       </c>
       <c r="P3" t="s">
@@ -4060,44 +4391,44 @@
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="50"/>
+      <c r="J4" s="50"/>
       <c r="M4" s="2" t="s">
         <v>19</v>
       </c>
       <c r="N4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O4" s="39"/>
+      <c r="O4" s="38"/>
       <c r="AA4" s="2"/>
       <c r="AB4" s="4"/>
-      <c r="AC4" s="44"/>
+      <c r="AC4" s="43"/>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
-      <c r="B5" s="38"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="38"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="50"/>
+      <c r="J5" s="50"/>
       <c r="M5" s="2" t="s">
         <v>20</v>
       </c>
       <c r="N5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="O5" s="39">
+      <c r="O5" s="38">
         <v>42</v>
       </c>
       <c r="P5" t="s">
@@ -4106,22 +4437,22 @@
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
-      <c r="B6" s="38"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="38"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="50"/>
+      <c r="I6" s="50"/>
+      <c r="J6" s="50"/>
       <c r="M6" s="2" t="s">
         <v>22</v>
       </c>
       <c r="N6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="O6" s="39">
+      <c r="O6" s="38">
         <v>28</v>
       </c>
       <c r="P6" t="s">
@@ -4132,40 +4463,40 @@
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
-      <c r="B7" s="38"/>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
-      <c r="J7" s="38"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="50"/>
       <c r="M7" s="2" t="s">
         <v>42</v>
       </c>
       <c r="N7" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="O7" s="40">
+      <c r="O7" s="39">
         <v>2.1</v>
       </c>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
-      <c r="B8" s="38"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="38"/>
-      <c r="J8" s="38"/>
+      <c r="B8" s="50"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="50"/>
+      <c r="H8" s="50"/>
+      <c r="I8" s="50"/>
+      <c r="J8" s="50"/>
       <c r="M8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="O8" s="39">
+      <c r="O8" s="38">
         <v>0.95</v>
       </c>
       <c r="AB8" s="2"/>
@@ -4173,19 +4504,19 @@
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="38"/>
-      <c r="J9" s="38"/>
+      <c r="B9" s="50"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="50"/>
+      <c r="I9" s="50"/>
+      <c r="J9" s="50"/>
       <c r="M9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="O9" s="39" t="s">
+      <c r="O9" s="38" t="s">
         <v>44</v>
       </c>
       <c r="AB9" s="2"/>
@@ -4193,22 +4524,22 @@
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
-      <c r="B10" s="38"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="38"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="50"/>
+      <c r="H10" s="50"/>
+      <c r="I10" s="50"/>
+      <c r="J10" s="50"/>
       <c r="M10" s="31" t="s">
         <v>16</v>
       </c>
       <c r="N10" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="O10" s="41">
+      <c r="O10" s="40">
         <f>1-O8</f>
         <v>5.0000000000000044E-2</v>
       </c>
@@ -4219,15 +4550,15 @@
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
-      <c r="B11" s="38"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
-      <c r="J11" s="38"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="50"/>
+      <c r="H11" s="50"/>
+      <c r="I11" s="50"/>
+      <c r="J11" s="50"/>
       <c r="M11" s="31" t="s">
         <v>46</v>
       </c>
@@ -4244,15 +4575,15 @@
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
-      <c r="B12" s="38"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
-      <c r="J12" s="38"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="50"/>
+      <c r="H12" s="50"/>
+      <c r="I12" s="50"/>
+      <c r="J12" s="50"/>
       <c r="M12" s="2" t="s">
         <v>73</v>
       </c>
@@ -4266,15 +4597,15 @@
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
-      <c r="B13" s="38"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="38"/>
-      <c r="J13" s="38"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="50"/>
+      <c r="H13" s="50"/>
+      <c r="I13" s="50"/>
+      <c r="J13" s="50"/>
       <c r="M13" s="2" t="s">
         <v>72</v>
       </c>
@@ -4472,7 +4803,7 @@
       <c r="N30" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="O30" s="47">
+      <c r="O30" s="46">
         <f>ROUND(O24,3)</f>
         <v>5.04</v>
       </c>
@@ -4490,7 +4821,7 @@
       <c r="N31" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="O31" s="48">
+      <c r="O31" s="47">
         <f>O11</f>
         <v>27</v>
       </c>
@@ -4499,7 +4830,7 @@
       <c r="R31" s="36"/>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B32" s="43">
+      <c r="B32" s="42">
         <f>O24</f>
         <v>5.0395263067896963</v>
       </c>
@@ -4508,7 +4839,7 @@
       <c r="N32" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="O32" s="49">
+      <c r="O32" s="48">
         <v>0</v>
       </c>
       <c r="P32" t="s">
@@ -4571,7 +4902,7 @@
       <c r="B37" s="1"/>
     </row>
     <row r="38" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B38" s="43"/>
+      <c r="B38" s="42"/>
       <c r="K38" s="1">
         <v>5</v>
       </c>
@@ -4580,7 +4911,7 @@
       </c>
     </row>
     <row r="39" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B39" s="43"/>
+      <c r="B39" s="42"/>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
       <c r="M39" s="34" t="str">
@@ -4589,7 +4920,7 @@
       </c>
     </row>
     <row r="40" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B40" s="43"/>
+      <c r="B40" s="42"/>
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
       <c r="M40" t="s">
@@ -4597,7 +4928,7 @@
       </c>
     </row>
     <row r="41" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B41" s="43"/>
+      <c r="B41" s="42"/>
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
     </row>
@@ -4615,17 +4946,17 @@
       <c r="A43" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B43" s="38" t="s">
+      <c r="B43" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="C43" s="38"/>
-      <c r="D43" s="38"/>
-      <c r="E43" s="38"/>
-      <c r="F43" s="38"/>
-      <c r="G43" s="38"/>
-      <c r="H43" s="38"/>
-      <c r="I43" s="38"/>
-      <c r="J43" s="38"/>
+      <c r="C43" s="50"/>
+      <c r="D43" s="50"/>
+      <c r="E43" s="50"/>
+      <c r="F43" s="50"/>
+      <c r="G43" s="50"/>
+      <c r="H43" s="50"/>
+      <c r="I43" s="50"/>
+      <c r="J43" s="50"/>
       <c r="K43" s="1">
         <v>1</v>
       </c>
@@ -4639,22 +4970,22 @@
     </row>
     <row r="44" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
-      <c r="B44" s="38"/>
-      <c r="C44" s="38"/>
-      <c r="D44" s="38"/>
-      <c r="E44" s="38"/>
-      <c r="F44" s="38"/>
-      <c r="G44" s="38"/>
-      <c r="H44" s="38"/>
-      <c r="I44" s="38"/>
-      <c r="J44" s="38"/>
+      <c r="B44" s="50"/>
+      <c r="C44" s="50"/>
+      <c r="D44" s="50"/>
+      <c r="E44" s="50"/>
+      <c r="F44" s="50"/>
+      <c r="G44" s="50"/>
+      <c r="H44" s="50"/>
+      <c r="I44" s="50"/>
+      <c r="J44" s="50"/>
       <c r="M44" s="2" t="s">
         <v>18</v>
       </c>
       <c r="N44" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O44" s="39">
+      <c r="O44" s="38">
         <v>60000</v>
       </c>
       <c r="P44" t="s">
@@ -4667,44 +4998,44 @@
     </row>
     <row r="45" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
-      <c r="B45" s="38"/>
-      <c r="C45" s="38"/>
-      <c r="D45" s="38"/>
-      <c r="E45" s="38"/>
-      <c r="F45" s="38"/>
-      <c r="G45" s="38"/>
-      <c r="H45" s="38"/>
-      <c r="I45" s="38"/>
-      <c r="J45" s="38"/>
+      <c r="B45" s="50"/>
+      <c r="C45" s="50"/>
+      <c r="D45" s="50"/>
+      <c r="E45" s="50"/>
+      <c r="F45" s="50"/>
+      <c r="G45" s="50"/>
+      <c r="H45" s="50"/>
+      <c r="I45" s="50"/>
+      <c r="J45" s="50"/>
       <c r="M45" s="2" t="s">
         <v>19</v>
       </c>
       <c r="N45" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O45" s="39"/>
+      <c r="O45" s="38"/>
       <c r="AA45" s="2"/>
       <c r="AB45" s="4"/>
-      <c r="AC45" s="44"/>
+      <c r="AC45" s="43"/>
     </row>
     <row r="46" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
-      <c r="B46" s="38"/>
-      <c r="C46" s="38"/>
-      <c r="D46" s="38"/>
-      <c r="E46" s="38"/>
-      <c r="F46" s="38"/>
-      <c r="G46" s="38"/>
-      <c r="H46" s="38"/>
-      <c r="I46" s="38"/>
-      <c r="J46" s="38"/>
+      <c r="B46" s="50"/>
+      <c r="C46" s="50"/>
+      <c r="D46" s="50"/>
+      <c r="E46" s="50"/>
+      <c r="F46" s="50"/>
+      <c r="G46" s="50"/>
+      <c r="H46" s="50"/>
+      <c r="I46" s="50"/>
+      <c r="J46" s="50"/>
       <c r="M46" s="2" t="s">
         <v>20</v>
       </c>
       <c r="N46" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="O46" s="39">
+      <c r="O46" s="38">
         <v>70000</v>
       </c>
       <c r="P46" t="s">
@@ -4713,22 +5044,22 @@
     </row>
     <row r="47" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A47" s="1"/>
-      <c r="B47" s="38"/>
-      <c r="C47" s="38"/>
-      <c r="D47" s="38"/>
-      <c r="E47" s="38"/>
-      <c r="F47" s="38"/>
-      <c r="G47" s="38"/>
-      <c r="H47" s="38"/>
-      <c r="I47" s="38"/>
-      <c r="J47" s="38"/>
+      <c r="B47" s="50"/>
+      <c r="C47" s="50"/>
+      <c r="D47" s="50"/>
+      <c r="E47" s="50"/>
+      <c r="F47" s="50"/>
+      <c r="G47" s="50"/>
+      <c r="H47" s="50"/>
+      <c r="I47" s="50"/>
+      <c r="J47" s="50"/>
       <c r="M47" s="2" t="s">
         <v>22</v>
       </c>
       <c r="N47" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="O47" s="39">
+      <c r="O47" s="38">
         <v>10</v>
       </c>
       <c r="P47" t="s">
@@ -4739,40 +5070,40 @@
     </row>
     <row r="48" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A48" s="1"/>
-      <c r="B48" s="38"/>
-      <c r="C48" s="38"/>
-      <c r="D48" s="38"/>
-      <c r="E48" s="38"/>
-      <c r="F48" s="38"/>
-      <c r="G48" s="38"/>
-      <c r="H48" s="38"/>
-      <c r="I48" s="38"/>
-      <c r="J48" s="38"/>
+      <c r="B48" s="50"/>
+      <c r="C48" s="50"/>
+      <c r="D48" s="50"/>
+      <c r="E48" s="50"/>
+      <c r="F48" s="50"/>
+      <c r="G48" s="50"/>
+      <c r="H48" s="50"/>
+      <c r="I48" s="50"/>
+      <c r="J48" s="50"/>
       <c r="M48" s="2" t="s">
         <v>42</v>
       </c>
       <c r="N48" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="O48" s="50">
+      <c r="O48" s="49">
         <v>10000</v>
       </c>
     </row>
     <row r="49" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A49" s="1"/>
-      <c r="B49" s="38"/>
-      <c r="C49" s="38"/>
-      <c r="D49" s="38"/>
-      <c r="E49" s="38"/>
-      <c r="F49" s="38"/>
-      <c r="G49" s="38"/>
-      <c r="H49" s="38"/>
-      <c r="I49" s="38"/>
-      <c r="J49" s="38"/>
+      <c r="B49" s="50"/>
+      <c r="C49" s="50"/>
+      <c r="D49" s="50"/>
+      <c r="E49" s="50"/>
+      <c r="F49" s="50"/>
+      <c r="G49" s="50"/>
+      <c r="H49" s="50"/>
+      <c r="I49" s="50"/>
+      <c r="J49" s="50"/>
       <c r="M49" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="O49" s="39">
+      <c r="O49" s="38">
         <v>0.95</v>
       </c>
       <c r="AB49" s="2"/>
@@ -4780,19 +5111,19 @@
     </row>
     <row r="50" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A50" s="1"/>
-      <c r="B50" s="38"/>
-      <c r="C50" s="38"/>
-      <c r="D50" s="38"/>
-      <c r="E50" s="38"/>
-      <c r="F50" s="38"/>
-      <c r="G50" s="38"/>
-      <c r="H50" s="38"/>
-      <c r="I50" s="38"/>
-      <c r="J50" s="38"/>
+      <c r="B50" s="50"/>
+      <c r="C50" s="50"/>
+      <c r="D50" s="50"/>
+      <c r="E50" s="50"/>
+      <c r="F50" s="50"/>
+      <c r="G50" s="50"/>
+      <c r="H50" s="50"/>
+      <c r="I50" s="50"/>
+      <c r="J50" s="50"/>
       <c r="M50" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="O50" s="39" t="s">
+      <c r="O50" s="38" t="s">
         <v>44</v>
       </c>
       <c r="AB50" s="2"/>
@@ -4800,22 +5131,22 @@
     </row>
     <row r="51" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A51" s="1"/>
-      <c r="B51" s="38"/>
-      <c r="C51" s="38"/>
-      <c r="D51" s="38"/>
-      <c r="E51" s="38"/>
-      <c r="F51" s="38"/>
-      <c r="G51" s="38"/>
-      <c r="H51" s="38"/>
-      <c r="I51" s="38"/>
-      <c r="J51" s="38"/>
+      <c r="B51" s="50"/>
+      <c r="C51" s="50"/>
+      <c r="D51" s="50"/>
+      <c r="E51" s="50"/>
+      <c r="F51" s="50"/>
+      <c r="G51" s="50"/>
+      <c r="H51" s="50"/>
+      <c r="I51" s="50"/>
+      <c r="J51" s="50"/>
       <c r="M51" s="31" t="s">
         <v>16</v>
       </c>
       <c r="N51" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="O51" s="41">
+      <c r="O51" s="40">
         <f>1-O49</f>
         <v>5.0000000000000044E-2</v>
       </c>
@@ -4826,15 +5157,15 @@
     </row>
     <row r="52" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A52" s="1"/>
-      <c r="B52" s="38"/>
-      <c r="C52" s="38"/>
-      <c r="D52" s="38"/>
-      <c r="E52" s="38"/>
-      <c r="F52" s="38"/>
-      <c r="G52" s="38"/>
-      <c r="H52" s="38"/>
-      <c r="I52" s="38"/>
-      <c r="J52" s="38"/>
+      <c r="B52" s="50"/>
+      <c r="C52" s="50"/>
+      <c r="D52" s="50"/>
+      <c r="E52" s="50"/>
+      <c r="F52" s="50"/>
+      <c r="G52" s="50"/>
+      <c r="H52" s="50"/>
+      <c r="I52" s="50"/>
+      <c r="J52" s="50"/>
       <c r="M52" s="31" t="s">
         <v>46</v>
       </c>
@@ -4851,15 +5182,15 @@
     </row>
     <row r="53" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A53" s="1"/>
-      <c r="B53" s="38"/>
-      <c r="C53" s="38"/>
-      <c r="D53" s="38"/>
-      <c r="E53" s="38"/>
-      <c r="F53" s="38"/>
-      <c r="G53" s="38"/>
-      <c r="H53" s="38"/>
-      <c r="I53" s="38"/>
-      <c r="J53" s="38"/>
+      <c r="B53" s="50"/>
+      <c r="C53" s="50"/>
+      <c r="D53" s="50"/>
+      <c r="E53" s="50"/>
+      <c r="F53" s="50"/>
+      <c r="G53" s="50"/>
+      <c r="H53" s="50"/>
+      <c r="I53" s="50"/>
+      <c r="J53" s="50"/>
       <c r="M53" s="2" t="s">
         <v>73</v>
       </c>
@@ -4873,15 +5204,15 @@
     </row>
     <row r="54" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A54" s="1"/>
-      <c r="B54" s="38"/>
-      <c r="C54" s="38"/>
-      <c r="D54" s="38"/>
-      <c r="E54" s="38"/>
-      <c r="F54" s="38"/>
-      <c r="G54" s="38"/>
-      <c r="H54" s="38"/>
-      <c r="I54" s="38"/>
-      <c r="J54" s="38"/>
+      <c r="B54" s="50"/>
+      <c r="C54" s="50"/>
+      <c r="D54" s="50"/>
+      <c r="E54" s="50"/>
+      <c r="F54" s="50"/>
+      <c r="G54" s="50"/>
+      <c r="H54" s="50"/>
+      <c r="I54" s="50"/>
+      <c r="J54" s="50"/>
       <c r="M54" s="2" t="s">
         <v>72</v>
       </c>
@@ -5079,7 +5410,7 @@
       <c r="N71" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="O71" s="47">
+      <c r="O71" s="46">
         <f>ROUND(O65,3)</f>
         <v>3.1619999999999999</v>
       </c>
@@ -5097,7 +5428,7 @@
       <c r="N72" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="O72" s="48">
+      <c r="O72" s="47">
         <f>O52</f>
         <v>9</v>
       </c>
@@ -5106,7 +5437,7 @@
       <c r="R72" s="36"/>
     </row>
     <row r="73" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B73" s="43">
+      <c r="B73" s="42">
         <f>O65</f>
         <v>3.1622776601683795</v>
       </c>
@@ -5115,7 +5446,7 @@
       <c r="N73" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="O73" s="49">
+      <c r="O73" s="48">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="P73" t="s">
@@ -5179,7 +5510,7 @@
       <c r="B78" s="1"/>
     </row>
     <row r="79" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B79" s="43"/>
+      <c r="B79" s="42"/>
       <c r="K79" s="1">
         <v>5</v>
       </c>
@@ -5255,17 +5586,17 @@
       <c r="A90" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B90" s="38" t="s">
+      <c r="B90" s="50" t="s">
         <v>89</v>
       </c>
-      <c r="C90" s="38"/>
-      <c r="D90" s="38"/>
-      <c r="E90" s="38"/>
-      <c r="F90" s="38"/>
-      <c r="G90" s="38"/>
-      <c r="H90" s="38"/>
-      <c r="I90" s="38"/>
-      <c r="J90" s="38"/>
+      <c r="C90" s="50"/>
+      <c r="D90" s="50"/>
+      <c r="E90" s="50"/>
+      <c r="F90" s="50"/>
+      <c r="G90" s="50"/>
+      <c r="H90" s="50"/>
+      <c r="I90" s="50"/>
+      <c r="J90" s="50"/>
       <c r="K90" s="1">
         <v>1</v>
       </c>
@@ -5287,22 +5618,22 @@
     </row>
     <row r="91" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A91" s="1"/>
-      <c r="B91" s="38"/>
-      <c r="C91" s="38"/>
-      <c r="D91" s="38"/>
-      <c r="E91" s="38"/>
-      <c r="F91" s="38"/>
-      <c r="G91" s="38"/>
-      <c r="H91" s="38"/>
-      <c r="I91" s="38"/>
-      <c r="J91" s="38"/>
+      <c r="B91" s="50"/>
+      <c r="C91" s="50"/>
+      <c r="D91" s="50"/>
+      <c r="E91" s="50"/>
+      <c r="F91" s="50"/>
+      <c r="G91" s="50"/>
+      <c r="H91" s="50"/>
+      <c r="I91" s="50"/>
+      <c r="J91" s="50"/>
       <c r="M91" s="2" t="s">
         <v>18</v>
       </c>
       <c r="N91" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O91" s="39">
+      <c r="O91" s="38">
         <v>1.4</v>
       </c>
       <c r="P91" t="s">
@@ -5327,22 +5658,22 @@
     </row>
     <row r="92" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A92" s="1"/>
-      <c r="B92" s="38"/>
-      <c r="C92" s="38"/>
-      <c r="D92" s="38"/>
-      <c r="E92" s="38"/>
-      <c r="F92" s="38"/>
-      <c r="G92" s="38"/>
-      <c r="H92" s="38"/>
-      <c r="I92" s="38"/>
-      <c r="J92" s="38"/>
+      <c r="B92" s="50"/>
+      <c r="C92" s="50"/>
+      <c r="D92" s="50"/>
+      <c r="E92" s="50"/>
+      <c r="F92" s="50"/>
+      <c r="G92" s="50"/>
+      <c r="H92" s="50"/>
+      <c r="I92" s="50"/>
+      <c r="J92" s="50"/>
       <c r="M92" s="2" t="s">
         <v>19</v>
       </c>
       <c r="N92" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O92" s="39"/>
+      <c r="O92" s="38"/>
       <c r="U92">
         <v>1.5</v>
       </c>
@@ -5356,28 +5687,28 @@
         <f>O98</f>
         <v>5.0000000000000044E-2</v>
       </c>
-      <c r="AC92" s="44" t="s">
+      <c r="AC92" s="43" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="93" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A93" s="1"/>
-      <c r="B93" s="38"/>
-      <c r="C93" s="38"/>
-      <c r="D93" s="38"/>
-      <c r="E93" s="38"/>
-      <c r="F93" s="38"/>
-      <c r="G93" s="38"/>
-      <c r="H93" s="38"/>
-      <c r="I93" s="38"/>
-      <c r="J93" s="38"/>
+      <c r="B93" s="50"/>
+      <c r="C93" s="50"/>
+      <c r="D93" s="50"/>
+      <c r="E93" s="50"/>
+      <c r="F93" s="50"/>
+      <c r="G93" s="50"/>
+      <c r="H93" s="50"/>
+      <c r="I93" s="50"/>
+      <c r="J93" s="50"/>
       <c r="M93" s="2" t="s">
         <v>20</v>
       </c>
       <c r="N93" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="O93" s="39">
+      <c r="O93" s="38">
         <f>AVERAGE(C96:C105)</f>
         <v>1.6000000000000003</v>
       </c>
@@ -5400,7 +5731,7 @@
       <c r="N94" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="O94" s="39">
+      <c r="O94" s="38">
         <f>COUNT(C96:C105)</f>
         <v>10</v>
       </c>
@@ -5428,7 +5759,7 @@
       <c r="N95" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="O95" s="50">
+      <c r="O95" s="49">
         <f>_xlfn.STDEV.S(C96:C105)</f>
         <v>0.21602468994692456</v>
       </c>
@@ -5448,7 +5779,7 @@
       <c r="M96" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="O96" s="39">
+      <c r="O96" s="38">
         <v>0.95</v>
       </c>
       <c r="U96">
@@ -5470,7 +5801,7 @@
       <c r="M97" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="O97" s="39" t="s">
+      <c r="O97" s="38" t="s">
         <v>44</v>
       </c>
       <c r="U97">
@@ -5495,7 +5826,7 @@
       <c r="N98" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="O98" s="41">
+      <c r="O98" s="40">
         <f>1-O96</f>
         <v>5.0000000000000044E-2</v>
       </c>
@@ -5797,7 +6128,7 @@
       <c r="N118" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="O118" s="47">
+      <c r="O118" s="46">
         <f>ROUND(O112,3)</f>
         <v>2.9279999999999999</v>
       </c>
@@ -5815,7 +6146,7 @@
       <c r="N119" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="O119" s="48">
+      <c r="O119" s="47">
         <f>O99</f>
         <v>9</v>
       </c>
@@ -5824,7 +6155,7 @@
       <c r="R119" s="36"/>
     </row>
     <row r="120" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B120" s="43">
+      <c r="B120" s="42">
         <f>O112</f>
         <v>2.9277002188456613</v>
       </c>
@@ -5833,7 +6164,7 @@
       <c r="N120" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="O120" s="49">
+      <c r="O120" s="48">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="P120" t="s">
@@ -5941,7 +6272,7 @@
       </c>
     </row>
     <row r="127" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B127" s="43">
+      <c r="B127" s="42">
         <f>AC96</f>
         <v>8.4099018161283654E-3</v>
       </c>
@@ -6078,17 +6409,17 @@
       <c r="A137" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B137" s="38" t="s">
+      <c r="B137" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="C137" s="38"/>
-      <c r="D137" s="38"/>
-      <c r="E137" s="38"/>
-      <c r="F137" s="38"/>
-      <c r="G137" s="38"/>
-      <c r="H137" s="38"/>
-      <c r="I137" s="38"/>
-      <c r="J137" s="38"/>
+      <c r="C137" s="50"/>
+      <c r="D137" s="50"/>
+      <c r="E137" s="50"/>
+      <c r="F137" s="50"/>
+      <c r="G137" s="50"/>
+      <c r="H137" s="50"/>
+      <c r="I137" s="50"/>
+      <c r="J137" s="50"/>
       <c r="K137" s="1">
         <v>1</v>
       </c>
@@ -6110,22 +6441,22 @@
     </row>
     <row r="138" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A138" s="1"/>
-      <c r="B138" s="38"/>
-      <c r="C138" s="38"/>
-      <c r="D138" s="38"/>
-      <c r="E138" s="38"/>
-      <c r="F138" s="38"/>
-      <c r="G138" s="38"/>
-      <c r="H138" s="38"/>
-      <c r="I138" s="38"/>
-      <c r="J138" s="38"/>
+      <c r="B138" s="50"/>
+      <c r="C138" s="50"/>
+      <c r="D138" s="50"/>
+      <c r="E138" s="50"/>
+      <c r="F138" s="50"/>
+      <c r="G138" s="50"/>
+      <c r="H138" s="50"/>
+      <c r="I138" s="50"/>
+      <c r="J138" s="50"/>
       <c r="M138" s="2" t="s">
         <v>18</v>
       </c>
       <c r="N138" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O138" s="39">
+      <c r="O138" s="38">
         <v>67</v>
       </c>
       <c r="P138" t="s">
@@ -6150,22 +6481,22 @@
     </row>
     <row r="139" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A139" s="1"/>
-      <c r="B139" s="38"/>
-      <c r="C139" s="38"/>
-      <c r="D139" s="38"/>
-      <c r="E139" s="38"/>
-      <c r="F139" s="38"/>
-      <c r="G139" s="38"/>
-      <c r="H139" s="38"/>
-      <c r="I139" s="38"/>
-      <c r="J139" s="38"/>
+      <c r="B139" s="50"/>
+      <c r="C139" s="50"/>
+      <c r="D139" s="50"/>
+      <c r="E139" s="50"/>
+      <c r="F139" s="50"/>
+      <c r="G139" s="50"/>
+      <c r="H139" s="50"/>
+      <c r="I139" s="50"/>
+      <c r="J139" s="50"/>
       <c r="M139" s="2" t="s">
         <v>19</v>
       </c>
       <c r="N139" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O139" s="39"/>
+      <c r="O139" s="38"/>
       <c r="U139">
         <v>51</v>
       </c>
@@ -6179,28 +6510,28 @@
         <f>O145</f>
         <v>5.0000000000000044E-2</v>
       </c>
-      <c r="AC139" s="44" t="s">
+      <c r="AC139" s="43" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="140" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A140" s="1"/>
-      <c r="B140" s="38"/>
-      <c r="C140" s="38"/>
-      <c r="D140" s="38"/>
-      <c r="E140" s="38"/>
-      <c r="F140" s="38"/>
-      <c r="G140" s="38"/>
-      <c r="H140" s="38"/>
-      <c r="I140" s="38"/>
-      <c r="J140" s="38"/>
+      <c r="B140" s="50"/>
+      <c r="C140" s="50"/>
+      <c r="D140" s="50"/>
+      <c r="E140" s="50"/>
+      <c r="F140" s="50"/>
+      <c r="G140" s="50"/>
+      <c r="H140" s="50"/>
+      <c r="I140" s="50"/>
+      <c r="J140" s="50"/>
       <c r="M140" s="2" t="s">
         <v>20</v>
       </c>
       <c r="N140" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="O140" s="39">
+      <c r="O140" s="38">
         <f>AVERAGE(C143:C154)</f>
         <v>82.5</v>
       </c>
@@ -6223,7 +6554,7 @@
       <c r="N141" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="O141" s="39">
+      <c r="O141" s="38">
         <f>COUNT(C143:C154)</f>
         <v>12</v>
       </c>
@@ -6251,7 +6582,7 @@
       <c r="N142" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="O142" s="50">
+      <c r="O142" s="49">
         <f>_xlfn.STDEV.S(C143:C154)</f>
         <v>59.492551099811116</v>
       </c>
@@ -6271,7 +6602,7 @@
       <c r="M143" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="O143" s="39">
+      <c r="O143" s="38">
         <v>0.95</v>
       </c>
       <c r="U143">
@@ -6293,7 +6624,7 @@
       <c r="M144" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="O144" s="39" t="s">
+      <c r="O144" s="38" t="s">
         <v>44</v>
       </c>
       <c r="U144">
@@ -6318,7 +6649,7 @@
       <c r="N145" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="O145" s="41">
+      <c r="O145" s="40">
         <f>1-O143</f>
         <v>5.0000000000000044E-2</v>
       </c>
@@ -6514,28 +6845,28 @@
       </c>
     </row>
     <row r="156" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B156" s="38" t="s">
+      <c r="B156" s="50" t="s">
         <v>94</v>
       </c>
-      <c r="C156" s="38"/>
-      <c r="D156" s="38"/>
-      <c r="E156" s="38"/>
-      <c r="F156" s="38"/>
-      <c r="G156" s="38"/>
-      <c r="H156" s="38"/>
-      <c r="I156" s="38"/>
-      <c r="J156" s="38"/>
+      <c r="C156" s="50"/>
+      <c r="D156" s="50"/>
+      <c r="E156" s="50"/>
+      <c r="F156" s="50"/>
+      <c r="G156" s="50"/>
+      <c r="H156" s="50"/>
+      <c r="I156" s="50"/>
+      <c r="J156" s="50"/>
     </row>
     <row r="157" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B157" s="38"/>
-      <c r="C157" s="38"/>
-      <c r="D157" s="38"/>
-      <c r="E157" s="38"/>
-      <c r="F157" s="38"/>
-      <c r="G157" s="38"/>
-      <c r="H157" s="38"/>
-      <c r="I157" s="38"/>
-      <c r="J157" s="38"/>
+      <c r="B157" s="50"/>
+      <c r="C157" s="50"/>
+      <c r="D157" s="50"/>
+      <c r="E157" s="50"/>
+      <c r="F157" s="50"/>
+      <c r="G157" s="50"/>
+      <c r="H157" s="50"/>
+      <c r="I157" s="50"/>
+      <c r="J157" s="50"/>
       <c r="K157" s="1">
         <v>3</v>
       </c>
@@ -6642,7 +6973,7 @@
       <c r="N165" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="O165" s="47">
+      <c r="O165" s="46">
         <f>ROUND(O159,3)</f>
         <v>0.90300000000000002</v>
       </c>
@@ -6661,7 +6992,7 @@
       <c r="N166" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="O166" s="48">
+      <c r="O166" s="47">
         <f>O146</f>
         <v>11</v>
       </c>
@@ -6675,7 +7006,7 @@
       <c r="N167" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="O167" s="49">
+      <c r="O167" s="48">
         <v>1</v>
       </c>
       <c r="P167" t="s">
@@ -6701,7 +7032,7 @@
       <c r="R168" s="36"/>
     </row>
     <row r="169" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B169" s="43">
+      <c r="B169" s="42">
         <f>O159</f>
         <v>0.90252601446781233</v>
       </c>
@@ -6805,7 +7136,7 @@
       </c>
     </row>
     <row r="176" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B176" s="43">
+      <c r="B176" s="42">
         <f>AC143</f>
         <v>0.19305705517763116</v>
       </c>
@@ -6935,17 +7266,17 @@
       <c r="A186" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B186" s="38" t="s">
+      <c r="B186" s="50" t="s">
         <v>121</v>
       </c>
-      <c r="C186" s="38"/>
-      <c r="D186" s="38"/>
-      <c r="E186" s="38"/>
-      <c r="F186" s="38"/>
-      <c r="G186" s="38"/>
-      <c r="H186" s="38"/>
-      <c r="I186" s="38"/>
-      <c r="J186" s="38"/>
+      <c r="C186" s="50"/>
+      <c r="D186" s="50"/>
+      <c r="E186" s="50"/>
+      <c r="F186" s="50"/>
+      <c r="G186" s="50"/>
+      <c r="H186" s="50"/>
+      <c r="I186" s="50"/>
+      <c r="J186" s="50"/>
       <c r="K186" s="1">
         <v>1</v>
       </c>
@@ -6967,22 +7298,22 @@
     </row>
     <row r="187" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A187" s="1"/>
-      <c r="B187" s="38"/>
-      <c r="C187" s="38"/>
-      <c r="D187" s="38"/>
-      <c r="E187" s="38"/>
-      <c r="F187" s="38"/>
-      <c r="G187" s="38"/>
-      <c r="H187" s="38"/>
-      <c r="I187" s="38"/>
-      <c r="J187" s="38"/>
+      <c r="B187" s="50"/>
+      <c r="C187" s="50"/>
+      <c r="D187" s="50"/>
+      <c r="E187" s="50"/>
+      <c r="F187" s="50"/>
+      <c r="G187" s="50"/>
+      <c r="H187" s="50"/>
+      <c r="I187" s="50"/>
+      <c r="J187" s="50"/>
       <c r="M187" s="2" t="s">
         <v>18</v>
       </c>
       <c r="N187" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O187" s="39">
+      <c r="O187" s="38">
         <v>8000</v>
       </c>
       <c r="P187" t="s">
@@ -7007,22 +7338,22 @@
     </row>
     <row r="188" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A188" s="1"/>
-      <c r="B188" s="38"/>
-      <c r="C188" s="38"/>
-      <c r="D188" s="38"/>
-      <c r="E188" s="38"/>
-      <c r="F188" s="38"/>
-      <c r="G188" s="38"/>
-      <c r="H188" s="38"/>
-      <c r="I188" s="38"/>
-      <c r="J188" s="38"/>
+      <c r="B188" s="50"/>
+      <c r="C188" s="50"/>
+      <c r="D188" s="50"/>
+      <c r="E188" s="50"/>
+      <c r="F188" s="50"/>
+      <c r="G188" s="50"/>
+      <c r="H188" s="50"/>
+      <c r="I188" s="50"/>
+      <c r="J188" s="50"/>
       <c r="M188" s="2" t="s">
         <v>19</v>
       </c>
       <c r="N188" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O188" s="39"/>
+      <c r="O188" s="38"/>
       <c r="U188">
         <v>7077</v>
       </c>
@@ -7036,28 +7367,28 @@
         <f>O194</f>
         <v>5.0000000000000044E-2</v>
       </c>
-      <c r="AC188" s="44" t="s">
+      <c r="AC188" s="43" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="189" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A189" s="1"/>
-      <c r="B189" s="38"/>
-      <c r="C189" s="38"/>
-      <c r="D189" s="38"/>
-      <c r="E189" s="38"/>
-      <c r="F189" s="38"/>
-      <c r="G189" s="38"/>
-      <c r="H189" s="38"/>
-      <c r="I189" s="38"/>
-      <c r="J189" s="38"/>
+      <c r="B189" s="50"/>
+      <c r="C189" s="50"/>
+      <c r="D189" s="50"/>
+      <c r="E189" s="50"/>
+      <c r="F189" s="50"/>
+      <c r="G189" s="50"/>
+      <c r="H189" s="50"/>
+      <c r="I189" s="50"/>
+      <c r="J189" s="50"/>
       <c r="M189" s="2" t="s">
         <v>20</v>
       </c>
       <c r="N189" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="O189" s="39">
+      <c r="O189" s="38">
         <f>AVERAGE(C192:C203)</f>
         <v>7163.583333333333</v>
       </c>
@@ -7080,7 +7411,7 @@
       <c r="N190" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="O190" s="39">
+      <c r="O190" s="38">
         <f>COUNT(C192:C203)</f>
         <v>12</v>
       </c>
@@ -7108,7 +7439,7 @@
       <c r="N191" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="O191" s="50">
+      <c r="O191" s="49">
         <f>_xlfn.STDEV.S(C192:C203)</f>
         <v>942.3700738354346</v>
       </c>
@@ -7128,7 +7459,7 @@
       <c r="M192" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="O192" s="39">
+      <c r="O192" s="38">
         <v>0.95</v>
       </c>
       <c r="U192">
@@ -7150,7 +7481,7 @@
       <c r="M193" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="O193" s="39" t="s">
+      <c r="O193" s="38" t="s">
         <v>36</v>
       </c>
       <c r="U193">
@@ -7175,7 +7506,7 @@
       <c r="N194" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="O194" s="41">
+      <c r="O194" s="40">
         <f>1-O192</f>
         <v>5.0000000000000044E-2</v>
       </c>
@@ -7371,26 +7702,26 @@
       </c>
     </row>
     <row r="205" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B205" s="38"/>
-      <c r="C205" s="38"/>
-      <c r="D205" s="38"/>
-      <c r="E205" s="38"/>
-      <c r="F205" s="38"/>
-      <c r="G205" s="38"/>
-      <c r="H205" s="38"/>
-      <c r="I205" s="38"/>
-      <c r="J205" s="38"/>
+      <c r="B205" s="50"/>
+      <c r="C205" s="50"/>
+      <c r="D205" s="50"/>
+      <c r="E205" s="50"/>
+      <c r="F205" s="50"/>
+      <c r="G205" s="50"/>
+      <c r="H205" s="50"/>
+      <c r="I205" s="50"/>
+      <c r="J205" s="50"/>
     </row>
     <row r="206" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="B206" s="38"/>
-      <c r="C206" s="38"/>
-      <c r="D206" s="38"/>
-      <c r="E206" s="38"/>
-      <c r="F206" s="38"/>
-      <c r="G206" s="38"/>
-      <c r="H206" s="38"/>
-      <c r="I206" s="38"/>
-      <c r="J206" s="38"/>
+      <c r="B206" s="50"/>
+      <c r="C206" s="50"/>
+      <c r="D206" s="50"/>
+      <c r="E206" s="50"/>
+      <c r="F206" s="50"/>
+      <c r="G206" s="50"/>
+      <c r="H206" s="50"/>
+      <c r="I206" s="50"/>
+      <c r="J206" s="50"/>
       <c r="K206" s="1">
         <v>3</v>
       </c>
@@ -7497,7 +7828,7 @@
       <c r="N214" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="O214" s="47">
+      <c r="O214" s="46">
         <f>ROUND(O208,3)</f>
         <v>-3.0750000000000002</v>
       </c>
@@ -7516,7 +7847,7 @@
       <c r="N215" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="O215" s="48">
+      <c r="O215" s="47">
         <f>O195</f>
         <v>11</v>
       </c>
@@ -7530,7 +7861,7 @@
       <c r="N216" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="O216" s="46">
+      <c r="O216" s="45">
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="P216" t="s">
@@ -7556,7 +7887,7 @@
       <c r="R217" s="36"/>
     </row>
     <row r="218" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B218" s="43">
+      <c r="B218" s="42">
         <f>O208</f>
         <v>-3.0746225993102945</v>
       </c>
@@ -7629,7 +7960,7 @@
       </c>
     </row>
     <row r="225" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B225" s="43">
+      <c r="B225" s="42">
         <f>AA192</f>
         <v>5.2861530427884924E-3</v>
       </c>
@@ -7791,17 +8122,17 @@
       <c r="A238" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B238" s="38" t="s">
+      <c r="B238" s="50" t="s">
         <v>124</v>
       </c>
-      <c r="C238" s="38"/>
-      <c r="D238" s="38"/>
-      <c r="E238" s="38"/>
-      <c r="F238" s="38"/>
-      <c r="G238" s="38"/>
-      <c r="H238" s="38"/>
-      <c r="I238" s="38"/>
-      <c r="J238" s="38"/>
+      <c r="C238" s="50"/>
+      <c r="D238" s="50"/>
+      <c r="E238" s="50"/>
+      <c r="F238" s="50"/>
+      <c r="G238" s="50"/>
+      <c r="H238" s="50"/>
+      <c r="I238" s="50"/>
+      <c r="J238" s="50"/>
       <c r="K238" s="1">
         <v>1</v>
       </c>
@@ -7823,22 +8154,22 @@
     </row>
     <row r="239" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A239" s="1"/>
-      <c r="B239" s="38"/>
-      <c r="C239" s="38"/>
-      <c r="D239" s="38"/>
-      <c r="E239" s="38"/>
-      <c r="F239" s="38"/>
-      <c r="G239" s="38"/>
-      <c r="H239" s="38"/>
-      <c r="I239" s="38"/>
-      <c r="J239" s="38"/>
+      <c r="B239" s="50"/>
+      <c r="C239" s="50"/>
+      <c r="D239" s="50"/>
+      <c r="E239" s="50"/>
+      <c r="F239" s="50"/>
+      <c r="G239" s="50"/>
+      <c r="H239" s="50"/>
+      <c r="I239" s="50"/>
+      <c r="J239" s="50"/>
       <c r="M239" s="2" t="s">
         <v>18</v>
       </c>
       <c r="N239" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O239" s="39">
+      <c r="O239" s="38">
         <v>6.5</v>
       </c>
       <c r="P239" t="s">
@@ -7863,22 +8194,22 @@
     </row>
     <row r="240" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A240" s="1"/>
-      <c r="B240" s="38"/>
-      <c r="C240" s="38"/>
-      <c r="D240" s="38"/>
-      <c r="E240" s="38"/>
-      <c r="F240" s="38"/>
-      <c r="G240" s="38"/>
-      <c r="H240" s="38"/>
-      <c r="I240" s="38"/>
-      <c r="J240" s="38"/>
+      <c r="B240" s="50"/>
+      <c r="C240" s="50"/>
+      <c r="D240" s="50"/>
+      <c r="E240" s="50"/>
+      <c r="F240" s="50"/>
+      <c r="G240" s="50"/>
+      <c r="H240" s="50"/>
+      <c r="I240" s="50"/>
+      <c r="J240" s="50"/>
       <c r="M240" s="2" t="s">
         <v>19</v>
       </c>
       <c r="N240" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O240" s="39"/>
+      <c r="O240" s="38"/>
       <c r="U240">
         <v>0</v>
       </c>
@@ -7892,28 +8223,28 @@
         <f>O246</f>
         <v>1.0000000000000009E-2</v>
       </c>
-      <c r="AC240" s="44" t="s">
+      <c r="AC240" s="43" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="241" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A241" s="1"/>
-      <c r="B241" s="38"/>
-      <c r="C241" s="38"/>
-      <c r="D241" s="38"/>
-      <c r="E241" s="38"/>
-      <c r="F241" s="38"/>
-      <c r="G241" s="38"/>
-      <c r="H241" s="38"/>
-      <c r="I241" s="38"/>
-      <c r="J241" s="38"/>
+      <c r="B241" s="50"/>
+      <c r="C241" s="50"/>
+      <c r="D241" s="50"/>
+      <c r="E241" s="50"/>
+      <c r="F241" s="50"/>
+      <c r="G241" s="50"/>
+      <c r="H241" s="50"/>
+      <c r="I241" s="50"/>
+      <c r="J241" s="50"/>
       <c r="M241" s="2" t="s">
         <v>20</v>
       </c>
       <c r="N241" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="O241" s="39">
+      <c r="O241" s="38">
         <f>AVERAGE(C244:C255)</f>
         <v>5.166666666666667</v>
       </c>
@@ -7936,7 +8267,7 @@
       <c r="N242" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="O242" s="39">
+      <c r="O242" s="38">
         <f>COUNT(C244:C255)</f>
         <v>12</v>
       </c>
@@ -7964,7 +8295,7 @@
       <c r="N243" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="O243" s="50">
+      <c r="O243" s="49">
         <f>_xlfn.STDEV.S(C244:C255)</f>
         <v>3.1574826950748234</v>
       </c>
@@ -7984,7 +8315,7 @@
       <c r="M244" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="O244" s="39">
+      <c r="O244" s="38">
         <v>0.99</v>
       </c>
       <c r="U244">
@@ -8006,7 +8337,7 @@
       <c r="M245" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="O245" s="39" t="s">
+      <c r="O245" s="38" t="s">
         <v>36</v>
       </c>
       <c r="U245">
@@ -8031,7 +8362,7 @@
       <c r="N246" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="O246" s="41">
+      <c r="O246" s="40">
         <f>1-O244</f>
         <v>1.0000000000000009E-2</v>
       </c>
@@ -8227,28 +8558,28 @@
       </c>
     </row>
     <row r="257" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B257" s="38" t="s">
+      <c r="B257" s="50" t="s">
         <v>125</v>
       </c>
-      <c r="C257" s="38"/>
-      <c r="D257" s="38"/>
-      <c r="E257" s="38"/>
-      <c r="F257" s="38"/>
-      <c r="G257" s="38"/>
-      <c r="H257" s="38"/>
-      <c r="I257" s="38"/>
-      <c r="J257" s="38"/>
+      <c r="C257" s="50"/>
+      <c r="D257" s="50"/>
+      <c r="E257" s="50"/>
+      <c r="F257" s="50"/>
+      <c r="G257" s="50"/>
+      <c r="H257" s="50"/>
+      <c r="I257" s="50"/>
+      <c r="J257" s="50"/>
     </row>
     <row r="258" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B258" s="38"/>
-      <c r="C258" s="38"/>
-      <c r="D258" s="38"/>
-      <c r="E258" s="38"/>
-      <c r="F258" s="38"/>
-      <c r="G258" s="38"/>
-      <c r="H258" s="38"/>
-      <c r="I258" s="38"/>
-      <c r="J258" s="38"/>
+      <c r="B258" s="50"/>
+      <c r="C258" s="50"/>
+      <c r="D258" s="50"/>
+      <c r="E258" s="50"/>
+      <c r="F258" s="50"/>
+      <c r="G258" s="50"/>
+      <c r="H258" s="50"/>
+      <c r="I258" s="50"/>
+      <c r="J258" s="50"/>
       <c r="K258" s="1">
         <v>3</v>
       </c>
@@ -8355,7 +8686,7 @@
       <c r="N266" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="O266" s="47">
+      <c r="O266" s="46">
         <f>ROUND(O260,3)</f>
         <v>-1.4630000000000001</v>
       </c>
@@ -8374,7 +8705,7 @@
       <c r="N267" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="O267" s="48">
+      <c r="O267" s="47">
         <f>O247</f>
         <v>11</v>
       </c>
@@ -8388,7 +8719,7 @@
       <c r="N268" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="O268" s="46">
+      <c r="O268" s="45">
         <v>0.05</v>
       </c>
       <c r="P268" t="s">
@@ -8414,7 +8745,7 @@
       <c r="R269" s="36"/>
     </row>
     <row r="270" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B270" s="43">
+      <c r="B270" s="42">
         <f>O260</f>
         <v>-1.4628115494414617</v>
       </c>
@@ -8487,7 +8818,7 @@
       </c>
     </row>
     <row r="277" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B277" s="43">
+      <c r="B277" s="42">
         <f>AA244</f>
         <v>8.5748432053813883E-2</v>
       </c>
@@ -8649,17 +8980,17 @@
       <c r="A290" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B290" s="38" t="s">
+      <c r="B290" s="50" t="s">
         <v>129</v>
       </c>
-      <c r="C290" s="38"/>
-      <c r="D290" s="38"/>
-      <c r="E290" s="38"/>
-      <c r="F290" s="38"/>
-      <c r="G290" s="38"/>
-      <c r="H290" s="38"/>
-      <c r="I290" s="38"/>
-      <c r="J290" s="38"/>
+      <c r="C290" s="50"/>
+      <c r="D290" s="50"/>
+      <c r="E290" s="50"/>
+      <c r="F290" s="50"/>
+      <c r="G290" s="50"/>
+      <c r="H290" s="50"/>
+      <c r="I290" s="50"/>
+      <c r="J290" s="50"/>
       <c r="K290" s="1">
         <v>1</v>
       </c>
@@ -8681,22 +9012,22 @@
     </row>
     <row r="291" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A291" s="1"/>
-      <c r="B291" s="38"/>
-      <c r="C291" s="38"/>
-      <c r="D291" s="38"/>
-      <c r="E291" s="38"/>
-      <c r="F291" s="38"/>
-      <c r="G291" s="38"/>
-      <c r="H291" s="38"/>
-      <c r="I291" s="38"/>
-      <c r="J291" s="38"/>
+      <c r="B291" s="50"/>
+      <c r="C291" s="50"/>
+      <c r="D291" s="50"/>
+      <c r="E291" s="50"/>
+      <c r="F291" s="50"/>
+      <c r="G291" s="50"/>
+      <c r="H291" s="50"/>
+      <c r="I291" s="50"/>
+      <c r="J291" s="50"/>
       <c r="M291" s="2" t="s">
         <v>18</v>
       </c>
       <c r="N291" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O291" s="39">
+      <c r="O291" s="38">
         <v>100</v>
       </c>
       <c r="P291" t="s">
@@ -8721,22 +9052,22 @@
     </row>
     <row r="292" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A292" s="1"/>
-      <c r="B292" s="38"/>
-      <c r="C292" s="38"/>
-      <c r="D292" s="38"/>
-      <c r="E292" s="38"/>
-      <c r="F292" s="38"/>
-      <c r="G292" s="38"/>
-      <c r="H292" s="38"/>
-      <c r="I292" s="38"/>
-      <c r="J292" s="38"/>
+      <c r="B292" s="50"/>
+      <c r="C292" s="50"/>
+      <c r="D292" s="50"/>
+      <c r="E292" s="50"/>
+      <c r="F292" s="50"/>
+      <c r="G292" s="50"/>
+      <c r="H292" s="50"/>
+      <c r="I292" s="50"/>
+      <c r="J292" s="50"/>
       <c r="M292" s="2" t="s">
         <v>19</v>
       </c>
       <c r="N292" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O292" s="39"/>
+      <c r="O292" s="38"/>
       <c r="U292">
         <v>120</v>
       </c>
@@ -8750,28 +9081,28 @@
         <f>O298</f>
         <v>5.0000000000000044E-2</v>
       </c>
-      <c r="AC292" s="44" t="s">
+      <c r="AC292" s="43" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="293" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A293" s="1"/>
-      <c r="B293" s="38"/>
-      <c r="C293" s="38"/>
-      <c r="D293" s="38"/>
-      <c r="E293" s="38"/>
-      <c r="F293" s="38"/>
-      <c r="G293" s="38"/>
-      <c r="H293" s="38"/>
-      <c r="I293" s="38"/>
-      <c r="J293" s="38"/>
+      <c r="B293" s="50"/>
+      <c r="C293" s="50"/>
+      <c r="D293" s="50"/>
+      <c r="E293" s="50"/>
+      <c r="F293" s="50"/>
+      <c r="G293" s="50"/>
+      <c r="H293" s="50"/>
+      <c r="I293" s="50"/>
+      <c r="J293" s="50"/>
       <c r="M293" s="2" t="s">
         <v>20</v>
       </c>
       <c r="N293" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="O293" s="39">
+      <c r="O293" s="38">
         <f>AVERAGE(C296:C310)</f>
         <v>109.4</v>
       </c>
@@ -8794,7 +9125,7 @@
       <c r="N294" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="O294" s="39">
+      <c r="O294" s="38">
         <f>COUNT(C296:C310)</f>
         <v>15</v>
       </c>
@@ -8822,7 +9153,7 @@
       <c r="N295" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="O295" s="50">
+      <c r="O295" s="49">
         <f>_xlfn.STDEV.S(C296:C310)</f>
         <v>9.9627879058596278</v>
       </c>
@@ -8842,7 +9173,7 @@
       <c r="M296" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="O296" s="39">
+      <c r="O296" s="38">
         <v>0.95</v>
       </c>
       <c r="U296">
@@ -8864,7 +9195,7 @@
       <c r="M297" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="O297" s="39" t="s">
+      <c r="O297" s="38" t="s">
         <v>44</v>
       </c>
       <c r="U297">
@@ -8889,7 +9220,7 @@
       <c r="N298" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="O298" s="41">
+      <c r="O298" s="40">
         <f>1-O296</f>
         <v>5.0000000000000044E-2</v>
       </c>
@@ -9133,17 +9464,17 @@
       </c>
     </row>
     <row r="313" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B313" s="38" t="s">
+      <c r="B313" s="50" t="s">
         <v>130</v>
       </c>
-      <c r="C313" s="38"/>
-      <c r="D313" s="38"/>
-      <c r="E313" s="38"/>
-      <c r="F313" s="38"/>
-      <c r="G313" s="38"/>
-      <c r="H313" s="38"/>
-      <c r="I313" s="38"/>
-      <c r="J313" s="38"/>
+      <c r="C313" s="50"/>
+      <c r="D313" s="50"/>
+      <c r="E313" s="50"/>
+      <c r="F313" s="50"/>
+      <c r="G313" s="50"/>
+      <c r="H313" s="50"/>
+      <c r="I313" s="50"/>
+      <c r="J313" s="50"/>
       <c r="M313" s="2" t="str">
         <f>ROUND(O312,4)&amp;O307</f>
         <v>3.6542 &gt; 1.761</v>
@@ -9154,15 +9485,15 @@
       </c>
     </row>
     <row r="314" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B314" s="38"/>
-      <c r="C314" s="38"/>
-      <c r="D314" s="38"/>
-      <c r="E314" s="38"/>
-      <c r="F314" s="38"/>
-      <c r="G314" s="38"/>
-      <c r="H314" s="38"/>
-      <c r="I314" s="38"/>
-      <c r="J314" s="38"/>
+      <c r="B314" s="50"/>
+      <c r="C314" s="50"/>
+      <c r="D314" s="50"/>
+      <c r="E314" s="50"/>
+      <c r="F314" s="50"/>
+      <c r="G314" s="50"/>
+      <c r="H314" s="50"/>
+      <c r="I314" s="50"/>
+      <c r="J314" s="50"/>
       <c r="M314" s="2" t="str">
         <f>IF(O297&lt;&gt;"both","",ROUND(O312,4)&amp;O308)</f>
         <v/>
@@ -9216,11 +9547,10 @@
       <c r="N318" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="O318" s="47">
+      <c r="O318" s="46">
         <f>ROUND(O312,3)</f>
         <v>3.6539999999999999</v>
       </c>
-      <c r="P318" s="9"/>
       <c r="Q318" s="36"/>
       <c r="R318" s="36"/>
     </row>
@@ -9239,7 +9569,7 @@
       <c r="N319" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="O319" s="48">
+      <c r="O319" s="47">
         <f>O299</f>
         <v>14</v>
       </c>
@@ -9253,7 +9583,7 @@
       <c r="N320" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="O320" s="46">
+      <c r="O320" s="45">
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="P320" t="s">
@@ -9297,26 +9627,33 @@
         <v>Reject the null hypothesis if p-value is &lt; 0.05</v>
       </c>
       <c r="N323" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="O323" s="85">
+        <f>1-_xlfn.T.DIST(O318,O294-1,TRUE)</f>
+        <v>1.302064927946156E-3</v>
+      </c>
+    </row>
+    <row r="324" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="N324" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="O323" s="25">
+      <c r="O324" s="25">
         <f>O298</f>
         <v>5.0000000000000044E-2</v>
-      </c>
-    </row>
-    <row r="324" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="N324" s="31" t="s">
-        <v>109</v>
-      </c>
-      <c r="O324" s="2" t="b">
-        <f>O321&lt;=O323</f>
-        <v>1</v>
       </c>
     </row>
     <row r="325" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B325" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="N325" s="31" t="s">
+        <v>109</v>
+      </c>
+      <c r="O325" s="2" t="b">
+        <f>O323&lt;=O324</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="326" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B326" s="2" t="s">
@@ -9344,7 +9681,7 @@
       <c r="K327" s="1"/>
       <c r="L327" s="1"/>
       <c r="M327" s="34" t="str">
-        <f>IFERROR(IF(O324,"Reject H0 ("&amp;O300&amp;")","Fail to reject H0 ("&amp;O300&amp;")"),"")</f>
+        <f>IFERROR(IF(O325,"Reject H0 ("&amp;O300&amp;")","Fail to reject H0 ("&amp;O300&amp;")"),"")</f>
         <v>Reject H0 (mu &lt;= 100)</v>
       </c>
       <c r="V327" t="s">
@@ -9436,7 +9773,7 @@
       <c r="X333" s="28"/>
     </row>
     <row r="334" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B334" s="43">
+      <c r="B334" s="42">
         <f>AA296</f>
         <v>1.3015427061343187E-3</v>
       </c>
@@ -9521,6 +9858,10 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B90:J93"/>
+    <mergeCell ref="B2:J13"/>
+    <mergeCell ref="B43:J54"/>
+    <mergeCell ref="B137:J140"/>
     <mergeCell ref="B313:J314"/>
     <mergeCell ref="B156:J157"/>
     <mergeCell ref="B186:J189"/>
@@ -9528,10 +9869,6 @@
     <mergeCell ref="B238:J241"/>
     <mergeCell ref="B257:J258"/>
     <mergeCell ref="B290:J293"/>
-    <mergeCell ref="B90:J93"/>
-    <mergeCell ref="B2:J13"/>
-    <mergeCell ref="B43:J54"/>
-    <mergeCell ref="B137:J140"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O50 O9 O97 O144 O193 O245 O297" xr:uid="{9ACDF434-4C30-4F1A-AC24-1569F7A428C3}">
@@ -9548,7 +9885,6 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
@@ -9562,13 +9898,13 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="36" x14ac:dyDescent="0.2">
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="44" t="s">
         <v>97</v>
       </c>
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="44" t="s">
         <v>98</v>
       </c>
-      <c r="D3" s="45" t="s">
+      <c r="D3" s="44" t="s">
         <v>99</v>
       </c>
     </row>
@@ -9745,13 +10081,799 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F21CE9CB-BEC3-4586-AB12-4373DD12DDCD}">
+  <dimension ref="A1:W30"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.7109375" customWidth="1"/>
+    <col min="10" max="10" width="7" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" customWidth="1"/>
+    <col min="16" max="16" width="2.42578125" customWidth="1"/>
+    <col min="17" max="17" width="7" customWidth="1"/>
+    <col min="18" max="19" width="5.140625" customWidth="1"/>
+    <col min="20" max="20" width="3.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B3" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="67" t="s">
+        <v>165</v>
+      </c>
+      <c r="K3" s="53"/>
+      <c r="L3" s="75"/>
+      <c r="M3" s="53"/>
+      <c r="N3" s="53"/>
+      <c r="O3" s="54"/>
+      <c r="Q3" s="67" t="s">
+        <v>164</v>
+      </c>
+      <c r="R3" s="53"/>
+      <c r="S3" s="53"/>
+      <c r="T3" s="53"/>
+      <c r="U3" s="53"/>
+      <c r="V3" s="53"/>
+      <c r="W3" s="54"/>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="50"/>
+      <c r="J4" s="55"/>
+      <c r="K4" s="76"/>
+      <c r="L4" s="77" t="s">
+        <v>147</v>
+      </c>
+      <c r="M4" s="92">
+        <v>100</v>
+      </c>
+      <c r="N4" s="56"/>
+      <c r="O4" s="57"/>
+      <c r="Q4" s="55"/>
+      <c r="R4" s="56"/>
+      <c r="S4" s="56"/>
+      <c r="T4" s="56"/>
+      <c r="U4" s="56"/>
+      <c r="V4" s="56"/>
+      <c r="W4" s="57"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="50"/>
+      <c r="J5" s="55"/>
+      <c r="K5" s="76"/>
+      <c r="L5" s="77" t="s">
+        <v>148</v>
+      </c>
+      <c r="M5" s="92">
+        <v>15</v>
+      </c>
+      <c r="N5" s="78" t="s">
+        <v>167</v>
+      </c>
+      <c r="O5" s="57"/>
+      <c r="Q5" s="55"/>
+      <c r="R5" s="71" t="s">
+        <v>166</v>
+      </c>
+      <c r="S5" s="70" t="s">
+        <v>161</v>
+      </c>
+      <c r="T5" s="56"/>
+      <c r="U5" s="65" t="s">
+        <v>163</v>
+      </c>
+      <c r="V5" s="56"/>
+      <c r="W5" s="57"/>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="50"/>
+      <c r="I6" s="50"/>
+      <c r="J6" s="55"/>
+      <c r="K6" s="76"/>
+      <c r="L6" s="77" t="s">
+        <v>151</v>
+      </c>
+      <c r="M6" s="92">
+        <v>0.05</v>
+      </c>
+      <c r="N6" s="56"/>
+      <c r="O6" s="57"/>
+      <c r="Q6" s="55"/>
+      <c r="R6" s="56">
+        <v>120</v>
+      </c>
+      <c r="S6" s="56">
+        <v>0</v>
+      </c>
+      <c r="T6" s="56"/>
+      <c r="U6" s="56"/>
+      <c r="V6" s="56"/>
+      <c r="W6" s="57"/>
+    </row>
+    <row r="7" spans="1:23" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="55"/>
+      <c r="K7" s="56"/>
+      <c r="L7" s="56"/>
+      <c r="M7" s="56"/>
+      <c r="N7" s="56"/>
+      <c r="O7" s="57"/>
+      <c r="Q7" s="55"/>
+      <c r="R7" s="56">
+        <v>108</v>
+      </c>
+      <c r="S7" s="56">
+        <v>0</v>
+      </c>
+      <c r="T7" s="56"/>
+      <c r="U7" s="72"/>
+      <c r="V7" s="71" t="s">
+        <v>131</v>
+      </c>
+      <c r="W7" s="73"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="B8" s="50"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="50"/>
+      <c r="H8" s="50"/>
+      <c r="I8" s="50"/>
+      <c r="J8" s="68" t="s">
+        <v>141</v>
+      </c>
+      <c r="K8" s="53"/>
+      <c r="L8" s="79" t="s">
+        <v>171</v>
+      </c>
+      <c r="M8" s="53" t="s">
+        <v>153</v>
+      </c>
+      <c r="N8" s="53"/>
+      <c r="O8" s="54"/>
+      <c r="Q8" s="55"/>
+      <c r="R8" s="56">
+        <v>120</v>
+      </c>
+      <c r="S8" s="56"/>
+      <c r="T8" s="56"/>
+      <c r="U8" s="69" t="s">
+        <v>54</v>
+      </c>
+      <c r="V8" s="28">
+        <v>109.4</v>
+      </c>
+      <c r="W8" s="74"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+      <c r="B9" s="50"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="50"/>
+      <c r="I9" s="50"/>
+      <c r="J9" s="55"/>
+      <c r="K9" s="56"/>
+      <c r="L9" s="80" t="s">
+        <v>172</v>
+      </c>
+      <c r="M9" s="56" t="s">
+        <v>154</v>
+      </c>
+      <c r="N9" s="56"/>
+      <c r="O9" s="57"/>
+      <c r="Q9" s="55"/>
+      <c r="R9" s="56">
+        <v>114</v>
+      </c>
+      <c r="S9" s="56"/>
+      <c r="T9" s="56"/>
+      <c r="U9" s="69" t="s">
+        <v>55</v>
+      </c>
+      <c r="V9" s="28">
+        <v>99.257142857142867</v>
+      </c>
+      <c r="W9" s="74"/>
+    </row>
+    <row r="10" spans="1:23" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="50"/>
+      <c r="H10" s="50"/>
+      <c r="I10" s="50"/>
+      <c r="J10" s="58"/>
+      <c r="K10" s="59"/>
+      <c r="L10" s="59"/>
+      <c r="M10" s="59"/>
+      <c r="N10" s="59"/>
+      <c r="O10" s="60"/>
+      <c r="P10" s="56"/>
+      <c r="Q10" s="55"/>
+      <c r="R10" s="56">
+        <v>118</v>
+      </c>
+      <c r="S10" s="56"/>
+      <c r="T10" s="56"/>
+      <c r="U10" s="69" t="s">
+        <v>56</v>
+      </c>
+      <c r="V10" s="28">
+        <v>15</v>
+      </c>
+      <c r="W10" s="74"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="68" t="s">
+        <v>142</v>
+      </c>
+      <c r="K11" s="53"/>
+      <c r="L11" s="53"/>
+      <c r="M11" s="53"/>
+      <c r="N11" s="53"/>
+      <c r="O11" s="54"/>
+      <c r="P11" s="56"/>
+      <c r="Q11" s="55"/>
+      <c r="R11" s="56">
+        <v>91</v>
+      </c>
+      <c r="S11" s="56"/>
+      <c r="T11" s="56"/>
+      <c r="U11" s="69" t="s">
+        <v>162</v>
+      </c>
+      <c r="V11" s="28">
+        <v>100</v>
+      </c>
+      <c r="W11" s="74"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="55"/>
+      <c r="K12" s="56"/>
+      <c r="L12" s="63" t="s">
+        <v>63</v>
+      </c>
+      <c r="M12" s="81">
+        <f>M6</f>
+        <v>0.05</v>
+      </c>
+      <c r="N12" s="56"/>
+      <c r="O12" s="57"/>
+      <c r="P12" s="56"/>
+      <c r="Q12" s="55"/>
+      <c r="R12" s="56">
+        <v>118</v>
+      </c>
+      <c r="S12" s="56"/>
+      <c r="T12" s="56"/>
+      <c r="U12" s="69" t="s">
+        <v>45</v>
+      </c>
+      <c r="V12" s="28">
+        <v>14</v>
+      </c>
+      <c r="W12" s="74"/>
+    </row>
+    <row r="13" spans="1:23" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1">
+        <v>120</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="62"/>
+      <c r="K13" s="59"/>
+      <c r="L13" s="59"/>
+      <c r="M13" s="59"/>
+      <c r="N13" s="59"/>
+      <c r="O13" s="60"/>
+      <c r="P13" s="56"/>
+      <c r="Q13" s="55"/>
+      <c r="R13" s="56">
+        <v>92</v>
+      </c>
+      <c r="S13" s="56"/>
+      <c r="T13" s="56"/>
+      <c r="U13" s="69" t="s">
+        <v>58</v>
+      </c>
+      <c r="V13" s="28">
+        <v>3.6542023977984592</v>
+      </c>
+      <c r="W13" s="74"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1">
+        <v>108</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="68" t="s">
+        <v>143</v>
+      </c>
+      <c r="K14" s="53"/>
+      <c r="L14" s="53"/>
+      <c r="M14" s="53"/>
+      <c r="N14" s="53"/>
+      <c r="O14" s="54"/>
+      <c r="P14" s="56"/>
+      <c r="Q14" s="55"/>
+      <c r="R14" s="56">
+        <v>104</v>
+      </c>
+      <c r="S14" s="56"/>
+      <c r="T14" s="56"/>
+      <c r="U14" s="69" t="s">
+        <v>59</v>
+      </c>
+      <c r="V14" s="86">
+        <v>1.3015427061343187E-3</v>
+      </c>
+      <c r="W14" s="74"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1">
+        <v>120</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="61"/>
+      <c r="K15" s="56"/>
+      <c r="L15" s="63" t="s">
+        <v>152</v>
+      </c>
+      <c r="M15" s="81" t="s">
+        <v>155</v>
+      </c>
+      <c r="N15" s="56"/>
+      <c r="O15" s="57"/>
+      <c r="P15" s="56"/>
+      <c r="Q15" s="55"/>
+      <c r="R15" s="56">
+        <v>104</v>
+      </c>
+      <c r="S15" s="56"/>
+      <c r="T15" s="56"/>
+      <c r="U15" s="69" t="s">
+        <v>60</v>
+      </c>
+      <c r="V15" s="28">
+        <v>1.7613101357748921</v>
+      </c>
+      <c r="W15" s="74"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1">
+        <v>114</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="61"/>
+      <c r="K16" s="56"/>
+      <c r="L16" s="63" t="s">
+        <v>149</v>
+      </c>
+      <c r="M16" s="88">
+        <f>AVERAGE(B13:B27)</f>
+        <v>109.4</v>
+      </c>
+      <c r="N16" s="78" t="s">
+        <v>168</v>
+      </c>
+      <c r="O16" s="57"/>
+      <c r="P16" s="56"/>
+      <c r="Q16" s="55"/>
+      <c r="R16" s="56">
+        <v>112</v>
+      </c>
+      <c r="S16" s="56"/>
+      <c r="T16" s="56"/>
+      <c r="U16" s="69"/>
+      <c r="V16" s="69" t="str">
+        <f>ROUND(V14,4)&amp;" &lt; "&amp;ROUND(M6,4)</f>
+        <v>0.0013 &lt; 0.05</v>
+      </c>
+      <c r="W16" s="74"/>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1">
+        <v>118</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="61"/>
+      <c r="K17" s="56"/>
+      <c r="L17" s="63" t="s">
+        <v>150</v>
+      </c>
+      <c r="M17" s="89">
+        <f>_xlfn.STDEV.S(B13:B27)</f>
+        <v>9.9627879058596278</v>
+      </c>
+      <c r="N17" s="78" t="s">
+        <v>169</v>
+      </c>
+      <c r="O17" s="57"/>
+      <c r="P17" s="56"/>
+      <c r="Q17" s="55"/>
+      <c r="R17" s="56">
+        <v>97</v>
+      </c>
+      <c r="S17" s="56"/>
+      <c r="T17" s="56"/>
+      <c r="U17" s="69"/>
+      <c r="V17" s="56" t="s">
+        <v>160</v>
+      </c>
+      <c r="W17" s="74"/>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1">
+        <v>91</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="55"/>
+      <c r="K18" s="56"/>
+      <c r="L18" s="63" t="s">
+        <v>156</v>
+      </c>
+      <c r="M18" s="89">
+        <f>(M16-M4)/(M17/SQRT(M5))</f>
+        <v>3.6542023977984592</v>
+      </c>
+      <c r="N18" s="78" t="s">
+        <v>175</v>
+      </c>
+      <c r="O18" s="57"/>
+      <c r="P18" s="56"/>
+      <c r="Q18" s="55"/>
+      <c r="R18" s="56">
+        <v>118</v>
+      </c>
+      <c r="S18" s="56"/>
+      <c r="T18" s="56"/>
+      <c r="U18" s="56"/>
+      <c r="W18" s="57"/>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1">
+        <v>118</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="55"/>
+      <c r="K19" s="56"/>
+      <c r="L19" s="63" t="s">
+        <v>45</v>
+      </c>
+      <c r="M19" s="81">
+        <f>M5-1</f>
+        <v>14</v>
+      </c>
+      <c r="N19" s="84" t="s">
+        <v>176</v>
+      </c>
+      <c r="O19" s="57"/>
+      <c r="P19" s="56"/>
+      <c r="Q19" s="55"/>
+      <c r="R19" s="56">
+        <v>108</v>
+      </c>
+      <c r="S19" s="56"/>
+      <c r="T19" s="56"/>
+      <c r="U19" s="56"/>
+      <c r="V19" s="65" t="s">
+        <v>158</v>
+      </c>
+      <c r="W19" s="57"/>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1">
+        <v>92</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="55"/>
+      <c r="K20" s="56"/>
+      <c r="L20" s="56">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="M20" s="81" t="s">
+        <v>157</v>
+      </c>
+      <c r="N20" s="81">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="O20" s="57"/>
+      <c r="P20" s="56"/>
+      <c r="Q20" s="55"/>
+      <c r="R20" s="56">
+        <v>117</v>
+      </c>
+      <c r="S20" s="56"/>
+      <c r="T20" s="56"/>
+      <c r="U20" s="56"/>
+      <c r="V20" s="56"/>
+      <c r="W20" s="57"/>
+    </row>
+    <row r="21" spans="1:23" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1">
+        <v>104</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="55"/>
+      <c r="K21" s="56"/>
+      <c r="L21" s="82" t="s">
+        <v>173</v>
+      </c>
+      <c r="M21" s="90">
+        <f>1-_xlfn.T.DIST(M18,M5-1,TRUE)</f>
+        <v>1.3015427061343621E-3</v>
+      </c>
+      <c r="N21" s="83" t="s">
+        <v>174</v>
+      </c>
+      <c r="O21" s="57"/>
+      <c r="P21" s="56"/>
+      <c r="Q21" s="64"/>
+      <c r="R21" s="59"/>
+      <c r="S21" s="59"/>
+      <c r="T21" s="59"/>
+      <c r="U21" s="59"/>
+      <c r="V21" s="59"/>
+      <c r="W21" s="60"/>
+    </row>
+    <row r="22" spans="1:23" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1">
+        <v>104</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="64"/>
+      <c r="K22" s="59"/>
+      <c r="L22" s="59"/>
+      <c r="M22" s="91" t="s">
+        <v>160</v>
+      </c>
+      <c r="N22" s="59"/>
+      <c r="O22" s="60"/>
+      <c r="P22" s="56"/>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="B23" s="1">
+        <v>112</v>
+      </c>
+      <c r="J23" s="68" t="s">
+        <v>144</v>
+      </c>
+      <c r="K23" s="53"/>
+      <c r="L23" s="53"/>
+      <c r="M23" s="53"/>
+      <c r="N23" s="53"/>
+      <c r="O23" s="54"/>
+      <c r="P23" s="56"/>
+      <c r="Q23" s="87" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="B24" s="1">
+        <v>97</v>
+      </c>
+      <c r="J24" s="61"/>
+      <c r="K24" s="56"/>
+      <c r="L24" s="65" t="s">
+        <v>158</v>
+      </c>
+      <c r="M24" s="56"/>
+      <c r="N24" s="56"/>
+      <c r="O24" s="57"/>
+      <c r="P24" s="56"/>
+    </row>
+    <row r="25" spans="1:23" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="1">
+        <v>118</v>
+      </c>
+      <c r="J25" s="55"/>
+      <c r="K25" s="56"/>
+      <c r="L25" s="51" t="s">
+        <v>159</v>
+      </c>
+      <c r="M25" s="51"/>
+      <c r="N25" s="51"/>
+      <c r="O25" s="57"/>
+      <c r="P25" s="56"/>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="B26" s="1">
+        <v>108</v>
+      </c>
+      <c r="J26" s="55"/>
+      <c r="K26" s="56"/>
+      <c r="L26" s="51"/>
+      <c r="M26" s="51"/>
+      <c r="N26" s="51"/>
+      <c r="O26" s="57"/>
+      <c r="P26" s="56"/>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="B27" s="1">
+        <v>117</v>
+      </c>
+      <c r="J27" s="55"/>
+      <c r="K27" s="56"/>
+      <c r="L27" s="51"/>
+      <c r="M27" s="51"/>
+      <c r="N27" s="51"/>
+      <c r="O27" s="57"/>
+      <c r="P27" s="56"/>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="J28" s="55"/>
+      <c r="K28" s="56"/>
+      <c r="L28" s="51"/>
+      <c r="M28" s="51"/>
+      <c r="N28" s="51"/>
+      <c r="O28" s="57"/>
+      <c r="P28" s="56"/>
+    </row>
+    <row r="29" spans="1:23" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J29" s="66"/>
+      <c r="K29" s="59"/>
+      <c r="L29" s="52"/>
+      <c r="M29" s="52"/>
+      <c r="N29" s="52"/>
+      <c r="O29" s="60"/>
+      <c r="P29" s="56"/>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="J30" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B3:I10"/>
+    <mergeCell ref="L25:N29"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BE672EF-43A3-4F8D-B7B5-88643A557C4D}">
   <dimension ref="A1:O42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
@@ -11291,12 +12413,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BB15AAC-DFF7-4683-BD98-0F2B1504CD5B}">
   <dimension ref="A1:AF42"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <sheetData>

</xml_diff>